<commit_message>
Finalize opcodes for v3
</commit_message>
<xml_diff>
--- a/opcode to control bits.xlsx
+++ b/opcode to control bits.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vjrai\Documents\SC8bCPU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92D8889C-FC9C-4834-A9D7-1C0E10B7C800}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E741263-B7BC-4B12-9689-3B5AB3040A4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="13875" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="v1" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3201" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3201" uniqueCount="112">
   <si>
     <t>Instruction</t>
   </si>
@@ -339,9 +339,6 @@
     <t>SWAPR</t>
   </si>
   <si>
-    <t>ASL</t>
-  </si>
-  <si>
     <t>ASR</t>
   </si>
   <si>
@@ -349,6 +346,39 @@
   </si>
   <si>
     <t>CSR</t>
+  </si>
+  <si>
+    <t>ADDD</t>
+  </si>
+  <si>
+    <t>ADDM</t>
+  </si>
+  <si>
+    <t>SUBM</t>
+  </si>
+  <si>
+    <t>SUBD</t>
+  </si>
+  <si>
+    <t>ANDM</t>
+  </si>
+  <si>
+    <t>ANDD</t>
+  </si>
+  <si>
+    <t>ORM</t>
+  </si>
+  <si>
+    <t>ORD</t>
+  </si>
+  <si>
+    <t>XORM</t>
+  </si>
+  <si>
+    <t>XORD</t>
+  </si>
+  <si>
+    <t>NOT</t>
   </si>
 </sst>
 </file>
@@ -370,12 +400,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -399,10 +435,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -685,9 +724,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X257"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T118" sqref="T118"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -14131,9 +14170,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E935C717-A0A0-4754-9512-CFF356DAFA88}">
   <dimension ref="A1:AA257"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Y21" sqref="Y21"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A228" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G258" sqref="G258"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -15053,59 +15092,59 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A34" s="1" t="s">
+    <row r="34" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A34" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B34" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C34" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="35" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A35" s="1" t="s">
+      <c r="C34" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="35" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A35" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B35" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C35" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="36" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A36" s="1" t="s">
+      <c r="C35" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="36" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A36" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B36" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C36" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="37" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A37" s="1" t="s">
+      <c r="C36" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="37" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A37" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B37" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C37" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D37" s="2" t="s">
+      <c r="C37" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D37" s="4" t="s">
         <v>29</v>
       </c>
     </row>
@@ -15447,7 +15486,7 @@
     </row>
     <row r="50" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A50" s="1" t="s">
-        <v>40</v>
+        <v>102</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>41</v>
@@ -15473,7 +15512,7 @@
     </row>
     <row r="51" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A51" s="1" t="s">
-        <v>40</v>
+        <v>102</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>41</v>
@@ -15505,7 +15544,7 @@
     </row>
     <row r="52" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A52" s="1" t="s">
-        <v>40</v>
+        <v>102</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>41</v>
@@ -15537,7 +15576,7 @@
     </row>
     <row r="53" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A53" s="1" t="s">
-        <v>40</v>
+        <v>102</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>41</v>
@@ -15575,7 +15614,7 @@
     </row>
     <row r="54" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A54" s="1" t="s">
-        <v>40</v>
+        <v>101</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>41</v>
@@ -15604,7 +15643,7 @@
     </row>
     <row r="55" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A55" s="1" t="s">
-        <v>40</v>
+        <v>101</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>41</v>
@@ -15639,7 +15678,7 @@
     </row>
     <row r="56" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A56" s="1" t="s">
-        <v>40</v>
+        <v>101</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>41</v>
@@ -15674,7 +15713,7 @@
     </row>
     <row r="57" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A57" s="1" t="s">
-        <v>40</v>
+        <v>101</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>41</v>
@@ -15995,7 +16034,7 @@
     </row>
     <row r="66" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A66" s="1" t="s">
-        <v>44</v>
+        <v>103</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>45</v>
@@ -16024,7 +16063,7 @@
     </row>
     <row r="67" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A67" s="1" t="s">
-        <v>44</v>
+        <v>103</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>45</v>
@@ -16059,7 +16098,7 @@
     </row>
     <row r="68" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A68" s="1" t="s">
-        <v>44</v>
+        <v>103</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>45</v>
@@ -16094,7 +16133,7 @@
     </row>
     <row r="69" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A69" s="1" t="s">
-        <v>44</v>
+        <v>103</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>45</v>
@@ -16135,7 +16174,7 @@
     </row>
     <row r="70" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A70" s="1" t="s">
-        <v>44</v>
+        <v>104</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>45</v>
@@ -16167,7 +16206,7 @@
     </row>
     <row r="71" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A71" s="1" t="s">
-        <v>44</v>
+        <v>104</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>45</v>
@@ -16205,7 +16244,7 @@
     </row>
     <row r="72" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A72" s="1" t="s">
-        <v>44</v>
+        <v>104</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>45</v>
@@ -16243,7 +16282,7 @@
     </row>
     <row r="73" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A73" s="1" t="s">
-        <v>44</v>
+        <v>104</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>45</v>
@@ -16729,619 +16768,619 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A86" s="1" t="s">
+    <row r="86" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A86" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="B86" s="1" t="s">
+      <c r="B86" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C86" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D86" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="87" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A87" s="1" t="s">
+      <c r="C86" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D86" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="87" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A87" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="B87" s="1" t="s">
+      <c r="B87" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C87" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D87" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="88" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A88" s="1" t="s">
+      <c r="C87" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D87" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="88" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A88" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="B88" s="1" t="s">
+      <c r="B88" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C88" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D88" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="89" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A89" s="1" t="s">
+      <c r="C88" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D88" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="89" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A89" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="B89" s="1" t="s">
+      <c r="B89" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C89" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D89" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="90" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A90" s="1" t="s">
+      <c r="C89" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D89" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="90" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A90" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="B90" s="1" t="s">
+      <c r="B90" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C90" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D90" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="91" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A91" s="1" t="s">
+      <c r="C90" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D90" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="91" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A91" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="B91" s="1" t="s">
+      <c r="B91" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C91" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D91" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="92" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A92" s="1" t="s">
+      <c r="C91" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D91" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="92" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A92" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="B92" s="1" t="s">
+      <c r="B92" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C92" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D92" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="93" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A93" s="1" t="s">
+      <c r="C92" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D92" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="93" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A93" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="B93" s="1" t="s">
+      <c r="B93" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C93" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D93" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="94" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A94" s="1" t="s">
+      <c r="C93" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D93" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="94" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A94" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="B94" s="1" t="s">
+      <c r="B94" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C94" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D94" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="95" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A95" s="1" t="s">
+      <c r="C94" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D94" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="95" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A95" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="B95" s="1" t="s">
+      <c r="B95" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C95" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D95" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="96" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A96" s="1" t="s">
+      <c r="C95" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D95" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="96" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A96" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="B96" s="1" t="s">
+      <c r="B96" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C96" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D96" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A97" s="1" t="s">
+      <c r="C96" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D96" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A97" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="B97" s="1" t="s">
+      <c r="B97" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C97" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D97" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A98" s="1" t="s">
+      <c r="C97" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D97" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A98" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="B98" s="1" t="s">
+      <c r="B98" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C98" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D98" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A99" s="1" t="s">
+      <c r="C98" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D98" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A99" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="B99" s="1" t="s">
+      <c r="B99" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C99" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D99" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A100" s="1" t="s">
+      <c r="C99" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D99" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A100" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="B100" s="1" t="s">
+      <c r="B100" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C100" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D100" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A101" s="1" t="s">
+      <c r="C100" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D100" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A101" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="B101" s="1" t="s">
+      <c r="B101" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C101" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D101" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A102" s="1" t="s">
+      <c r="C101" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D101" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A102" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="B102" s="1" t="s">
+      <c r="B102" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C102" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D102" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A103" s="1" t="s">
+      <c r="C102" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D102" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A103" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="B103" s="1" t="s">
+      <c r="B103" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C103" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D103" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A104" s="1" t="s">
+      <c r="C103" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D103" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A104" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="B104" s="1" t="s">
+      <c r="B104" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C104" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D104" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A105" s="1" t="s">
+      <c r="C104" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D104" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A105" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="B105" s="1" t="s">
+      <c r="B105" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C105" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D105" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A106" s="1" t="s">
+      <c r="C105" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D105" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A106" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="B106" s="1" t="s">
+      <c r="B106" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C106" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D106" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A107" s="1" t="s">
+      <c r="C106" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D106" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A107" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="B107" s="1" t="s">
+      <c r="B107" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C107" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D107" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A108" s="1" t="s">
+      <c r="C107" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D107" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A108" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="B108" s="1" t="s">
+      <c r="B108" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C108" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D108" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A109" s="1" t="s">
+      <c r="C108" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D108" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A109" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="B109" s="1" t="s">
+      <c r="B109" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C109" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D109" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A110" s="1" t="s">
+      <c r="C109" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D109" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A110" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="B110" s="1" t="s">
+      <c r="B110" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C110" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D110" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A111" s="1" t="s">
+      <c r="C110" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D110" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A111" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="B111" s="1" t="s">
+      <c r="B111" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C111" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D111" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A112" s="1" t="s">
+      <c r="C111" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D111" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A112" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="B112" s="1" t="s">
+      <c r="B112" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C112" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D112" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A113" s="1" t="s">
+      <c r="C112" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D112" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A113" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="B113" s="1" t="s">
+      <c r="B113" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C113" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D113" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A114" s="1" t="s">
+      <c r="C113" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D113" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A114" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B114" s="1" t="s">
+      <c r="B114" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C114" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D114" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A115" s="1" t="s">
+      <c r="C114" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D114" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A115" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B115" s="1" t="s">
+      <c r="B115" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C115" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D115" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A116" s="1" t="s">
+      <c r="C115" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D115" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A116" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B116" s="1" t="s">
+      <c r="B116" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C116" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D116" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A117" s="1" t="s">
+      <c r="C116" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D116" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A117" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B117" s="1" t="s">
+      <c r="B117" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C117" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D117" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A118" s="1" t="s">
+      <c r="C117" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D117" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A118" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B118" s="1" t="s">
+      <c r="B118" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C118" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D118" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A119" s="1" t="s">
+      <c r="C118" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D118" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A119" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B119" s="1" t="s">
+      <c r="B119" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C119" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D119" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A120" s="1" t="s">
+      <c r="C119" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D119" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A120" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B120" s="1" t="s">
+      <c r="B120" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C120" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D120" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A121" s="1" t="s">
+      <c r="C120" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D120" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A121" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B121" s="1" t="s">
+      <c r="B121" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C121" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D121" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A122" s="1" t="s">
+      <c r="C121" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D121" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A122" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B122" s="1" t="s">
+      <c r="B122" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C122" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D122" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A123" s="1" t="s">
+      <c r="C122" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D122" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A123" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B123" s="1" t="s">
+      <c r="B123" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C123" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D123" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A124" s="1" t="s">
+      <c r="C123" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D123" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A124" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B124" s="1" t="s">
+      <c r="B124" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C124" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D124" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A125" s="1" t="s">
+      <c r="C124" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D124" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A125" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B125" s="1" t="s">
+      <c r="B125" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C125" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D125" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A126" s="1" t="s">
+      <c r="C125" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D125" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A126" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B126" s="1" t="s">
+      <c r="B126" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C126" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D126" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A127" s="1" t="s">
+      <c r="C126" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D126" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A127" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B127" s="1" t="s">
+      <c r="B127" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C127" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D127" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A128" s="1" t="s">
+      <c r="C127" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D127" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A128" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B128" s="1" t="s">
+      <c r="B128" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C128" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D128" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="129" spans="1:24" x14ac:dyDescent="0.45">
-      <c r="A129" s="1" t="s">
+      <c r="C128" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D128" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="129" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A129" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B129" s="1" t="s">
+      <c r="B129" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C129" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D129" s="2" t="s">
+      <c r="C129" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D129" s="4" t="s">
         <v>29</v>
       </c>
     </row>
@@ -18309,171 +18348,171 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A162" s="1" t="s">
+    <row r="162" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A162" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="B162" s="1" t="s">
+      <c r="B162" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C162" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D162" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="163" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A163" s="1" t="s">
+      <c r="C162" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D162" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="163" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A163" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="B163" s="1" t="s">
+      <c r="B163" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C163" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D163" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="164" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A164" s="1" t="s">
+      <c r="C163" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D163" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="164" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A164" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="B164" s="1" t="s">
+      <c r="B164" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C164" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D164" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="165" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A165" s="1" t="s">
+      <c r="C164" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D164" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="165" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A165" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="B165" s="1" t="s">
+      <c r="B165" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C165" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D165" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="166" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A166" s="1" t="s">
+      <c r="C165" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D165" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="166" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A166" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="B166" s="1" t="s">
+      <c r="B166" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C166" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D166" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="167" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A167" s="1" t="s">
+      <c r="C166" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D166" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="167" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A167" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="B167" s="1" t="s">
+      <c r="B167" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C167" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D167" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="168" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A168" s="1" t="s">
+      <c r="C167" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D167" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="168" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A168" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="B168" s="1" t="s">
+      <c r="B168" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C168" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D168" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="169" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A169" s="1" t="s">
+      <c r="C168" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D168" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="169" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A169" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="B169" s="1" t="s">
+      <c r="B169" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C169" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D169" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="170" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A170" s="1" t="s">
+      <c r="C169" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D169" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="170" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A170" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="B170" s="1" t="s">
+      <c r="B170" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C170" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D170" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="171" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A171" s="1" t="s">
+      <c r="C170" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D170" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="171" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A171" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="B171" s="1" t="s">
+      <c r="B171" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C171" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D171" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="172" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A172" s="1" t="s">
+      <c r="C171" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D171" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="172" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A172" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="B172" s="1" t="s">
+      <c r="B172" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C172" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D172" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="173" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A173" s="1" t="s">
+      <c r="C172" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D172" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="173" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A173" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="B173" s="1" t="s">
+      <c r="B173" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C173" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D173" s="2" t="s">
+      <c r="C173" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D173" s="4" t="s">
         <v>29</v>
       </c>
     </row>
@@ -18879,7 +18918,7 @@
     </row>
     <row r="194" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A194" s="1" t="s">
-        <v>68</v>
+        <v>105</v>
       </c>
       <c r="B194" s="1" t="s">
         <v>69</v>
@@ -18905,7 +18944,7 @@
     </row>
     <row r="195" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A195" s="1" t="s">
-        <v>68</v>
+        <v>105</v>
       </c>
       <c r="B195" s="1" t="s">
         <v>69</v>
@@ -18937,7 +18976,7 @@
     </row>
     <row r="196" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A196" s="1" t="s">
-        <v>68</v>
+        <v>105</v>
       </c>
       <c r="B196" s="1" t="s">
         <v>69</v>
@@ -18969,7 +19008,7 @@
     </row>
     <row r="197" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A197" s="1" t="s">
-        <v>68</v>
+        <v>105</v>
       </c>
       <c r="B197" s="1" t="s">
         <v>69</v>
@@ -19007,7 +19046,7 @@
     </row>
     <row r="198" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A198" s="1" t="s">
-        <v>68</v>
+        <v>106</v>
       </c>
       <c r="B198" s="1" t="s">
         <v>69</v>
@@ -19036,7 +19075,7 @@
     </row>
     <row r="199" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A199" s="1" t="s">
-        <v>68</v>
+        <v>106</v>
       </c>
       <c r="B199" s="1" t="s">
         <v>69</v>
@@ -19071,7 +19110,7 @@
     </row>
     <row r="200" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A200" s="1" t="s">
-        <v>68</v>
+        <v>106</v>
       </c>
       <c r="B200" s="1" t="s">
         <v>69</v>
@@ -19106,7 +19145,7 @@
     </row>
     <row r="201" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A201" s="1" t="s">
-        <v>68</v>
+        <v>106</v>
       </c>
       <c r="B201" s="1" t="s">
         <v>69</v>
@@ -19427,7 +19466,7 @@
     </row>
     <row r="210" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A210" s="1" t="s">
-        <v>72</v>
+        <v>107</v>
       </c>
       <c r="B210" s="1" t="s">
         <v>73</v>
@@ -19453,7 +19492,7 @@
     </row>
     <row r="211" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A211" s="1" t="s">
-        <v>72</v>
+        <v>107</v>
       </c>
       <c r="B211" s="1" t="s">
         <v>73</v>
@@ -19485,7 +19524,7 @@
     </row>
     <row r="212" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A212" s="1" t="s">
-        <v>72</v>
+        <v>107</v>
       </c>
       <c r="B212" s="1" t="s">
         <v>73</v>
@@ -19517,7 +19556,7 @@
     </row>
     <row r="213" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A213" s="1" t="s">
-        <v>72</v>
+        <v>107</v>
       </c>
       <c r="B213" s="1" t="s">
         <v>73</v>
@@ -19555,7 +19594,7 @@
     </row>
     <row r="214" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A214" s="1" t="s">
-        <v>72</v>
+        <v>108</v>
       </c>
       <c r="B214" s="1" t="s">
         <v>73</v>
@@ -19584,7 +19623,7 @@
     </row>
     <row r="215" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A215" s="1" t="s">
-        <v>72</v>
+        <v>108</v>
       </c>
       <c r="B215" s="1" t="s">
         <v>73</v>
@@ -19619,7 +19658,7 @@
     </row>
     <row r="216" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A216" s="1" t="s">
-        <v>72</v>
+        <v>108</v>
       </c>
       <c r="B216" s="1" t="s">
         <v>73</v>
@@ -19654,7 +19693,7 @@
     </row>
     <row r="217" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A217" s="1" t="s">
-        <v>72</v>
+        <v>108</v>
       </c>
       <c r="B217" s="1" t="s">
         <v>73</v>
@@ -19978,7 +20017,7 @@
     </row>
     <row r="226" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A226" s="1" t="s">
-        <v>77</v>
+        <v>109</v>
       </c>
       <c r="B226" s="1" t="s">
         <v>78</v>
@@ -20007,7 +20046,7 @@
     </row>
     <row r="227" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A227" s="1" t="s">
-        <v>77</v>
+        <v>109</v>
       </c>
       <c r="B227" s="1" t="s">
         <v>78</v>
@@ -20042,7 +20081,7 @@
     </row>
     <row r="228" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A228" s="1" t="s">
-        <v>77</v>
+        <v>109</v>
       </c>
       <c r="B228" s="1" t="s">
         <v>78</v>
@@ -20077,7 +20116,7 @@
     </row>
     <row r="229" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A229" s="1" t="s">
-        <v>77</v>
+        <v>109</v>
       </c>
       <c r="B229" s="1" t="s">
         <v>78</v>
@@ -20118,7 +20157,7 @@
     </row>
     <row r="230" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A230" s="1" t="s">
-        <v>77</v>
+        <v>110</v>
       </c>
       <c r="B230" s="1" t="s">
         <v>78</v>
@@ -20150,7 +20189,7 @@
     </row>
     <row r="231" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A231" s="1" t="s">
-        <v>77</v>
+        <v>110</v>
       </c>
       <c r="B231" s="1" t="s">
         <v>78</v>
@@ -20188,7 +20227,7 @@
     </row>
     <row r="232" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A232" s="1" t="s">
-        <v>77</v>
+        <v>110</v>
       </c>
       <c r="B232" s="1" t="s">
         <v>78</v>
@@ -20226,7 +20265,7 @@
     </row>
     <row r="233" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A233" s="1" t="s">
-        <v>77</v>
+        <v>110</v>
       </c>
       <c r="B233" s="1" t="s">
         <v>78</v>
@@ -20572,227 +20611,227 @@
         <v>1</v>
       </c>
     </row>
-    <row r="242" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A242" s="1" t="s">
+    <row r="242" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A242" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B242" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C242" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D242" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="243" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A243" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B243" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C243" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D243" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="244" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A244" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B244" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C244" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D244" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="245" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A245" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B245" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C245" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D245" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="246" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A246" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="B242" s="1" t="s">
+      <c r="B246" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="C242" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D242" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="243" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A243" s="1" t="s">
+      <c r="C246" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D246" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="247" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A247" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="B243" s="1" t="s">
+      <c r="B247" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="C243" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D243" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="244" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A244" s="1" t="s">
+      <c r="C247" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D247" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="248" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A248" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="B244" s="1" t="s">
+      <c r="B248" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="C244" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D244" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="245" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A245" s="1" t="s">
+      <c r="C248" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D248" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="249" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A249" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="B245" s="1" t="s">
+      <c r="B249" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="C245" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D245" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="246" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A246" s="1" t="s">
+      <c r="C249" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D249" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="250" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A250" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="B246" s="1" t="s">
+      <c r="B250" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="C246" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D246" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="247" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A247" s="1" t="s">
+      <c r="C250" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D250" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="251" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A251" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="B247" s="1" t="s">
+      <c r="B251" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="C247" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D247" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="248" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A248" s="1" t="s">
+      <c r="C251" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D251" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="252" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A252" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="B248" s="1" t="s">
+      <c r="B252" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="C248" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D248" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="249" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A249" s="1" t="s">
+      <c r="C252" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D252" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="253" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A253" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="B249" s="1" t="s">
+      <c r="B253" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="C249" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D249" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="250" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A250" s="1" t="s">
+      <c r="C253" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D253" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="254" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A254" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B250" s="1" t="s">
+      <c r="B254" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="C250" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D250" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="251" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A251" s="1" t="s">
+      <c r="C254" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D254" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="255" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A255" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B251" s="1" t="s">
+      <c r="B255" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="C251" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D251" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="252" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A252" s="1" t="s">
+      <c r="C255" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D255" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="256" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A256" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B252" s="1" t="s">
+      <c r="B256" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="C252" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D252" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="253" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A253" s="1" t="s">
+      <c r="C256" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D256" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="257" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A257" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B253" s="1" t="s">
+      <c r="B257" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="C253" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D253" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="254" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A254" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="B254" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C254" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D254" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="255" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A255" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="B255" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C255" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D255" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="256" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A256" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="B256" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C256" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D256" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="257" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A257" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="B257" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C257" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D257" s="2" t="s">
+      <c r="C257" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D257" s="4" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>

<commit_message>
CPU v3 started. Control unit & MReg adjusted. ALU left
</commit_message>
<xml_diff>
--- a/opcode to control bits.xlsx
+++ b/opcode to control bits.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vjrai\Documents\SC8bCPU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41BE432A-0F16-41C7-8F19-CB0405F44ABA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2710C16F-B066-4BEB-9302-DC0F8E9FC3AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="13875" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'v1'!$A$1:$X$257</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'v2'!$A$1:$AA$257</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'v3'!$A$1:$AB$257</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'v3'!$A$1:$AC$257</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3202" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3203" uniqueCount="113">
   <si>
     <t>Instruction</t>
   </si>
@@ -403,18 +403,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -438,16 +432,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -14174,13 +14162,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E935C717-A0A0-4754-9512-CFF356DAFA88}">
-  <dimension ref="A1:AB257"/>
+  <dimension ref="A1:AC257"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E20" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F39" sqref="F39"/>
+      <selection pane="bottomRight" activeCell="E173" sqref="E173"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -14207,7 +14195,7 @@
     <col min="28" max="28" width="7.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -14292,8 +14280,11 @@
       <c r="AB1" s="1" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.45">
+      <c r="AC1" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>24</v>
       </c>
@@ -14310,7 +14301,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>24</v>
       </c>
@@ -14327,7 +14318,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>24</v>
       </c>
@@ -14344,7 +14335,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>24</v>
       </c>
@@ -14361,7 +14352,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>52</v>
       </c>
@@ -14387,7 +14378,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>52</v>
       </c>
@@ -14416,7 +14407,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>52</v>
       </c>
@@ -14445,7 +14436,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>52</v>
       </c>
@@ -14477,7 +14468,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>54</v>
       </c>
@@ -14497,7 +14488,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>54</v>
       </c>
@@ -14520,7 +14511,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>54</v>
       </c>
@@ -14543,7 +14534,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
         <v>54</v>
       </c>
@@ -14569,7 +14560,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
         <v>81</v>
       </c>
@@ -14583,7 +14574,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
         <v>81</v>
       </c>
@@ -14597,7 +14588,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>81</v>
       </c>
@@ -15102,204 +15093,132 @@
       </c>
     </row>
     <row r="34" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="A34" s="6" t="s">
+      <c r="A34" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="B34" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C34" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D34" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E34" s="8">
-        <v>1</v>
-      </c>
-      <c r="F34" s="8"/>
-      <c r="G34" s="8">
-        <v>1</v>
-      </c>
-      <c r="H34" s="8"/>
-      <c r="I34" s="8"/>
-      <c r="J34" s="8"/>
-      <c r="K34" s="8"/>
-      <c r="L34" s="8"/>
-      <c r="M34" s="8"/>
-      <c r="N34" s="8"/>
-      <c r="O34" s="8"/>
-      <c r="P34" s="8"/>
-      <c r="Q34" s="8"/>
-      <c r="R34" s="8"/>
-      <c r="S34" s="8"/>
-      <c r="T34" s="8"/>
-      <c r="U34" s="8"/>
-      <c r="V34" s="8">
-        <v>1</v>
-      </c>
-      <c r="W34" s="8"/>
-      <c r="X34" s="8"/>
-      <c r="Y34" s="8">
-        <v>1</v>
-      </c>
-      <c r="Z34" s="8"/>
-      <c r="AA34" s="8"/>
-      <c r="AB34" s="8"/>
+      <c r="C34" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+      <c r="G34">
+        <v>1</v>
+      </c>
+      <c r="V34">
+        <v>1</v>
+      </c>
+      <c r="Y34">
+        <v>1</v>
+      </c>
     </row>
     <row r="35" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="A35" s="6" t="s">
+      <c r="A35" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B35" s="6" t="s">
+      <c r="B35" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C35" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D35" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E35" s="8">
-        <v>1</v>
-      </c>
-      <c r="F35" s="8"/>
-      <c r="G35" s="8">
-        <v>1</v>
-      </c>
-      <c r="H35" s="8"/>
-      <c r="I35" s="8">
-        <v>1</v>
-      </c>
-      <c r="J35" s="8"/>
-      <c r="K35" s="8"/>
-      <c r="L35" s="8">
-        <v>1</v>
-      </c>
-      <c r="M35" s="8"/>
-      <c r="N35" s="8"/>
-      <c r="O35" s="8"/>
-      <c r="P35" s="8"/>
-      <c r="Q35" s="8"/>
-      <c r="R35" s="8"/>
-      <c r="S35" s="8"/>
-      <c r="T35" s="8"/>
-      <c r="U35" s="8"/>
-      <c r="V35" s="8">
-        <v>1</v>
-      </c>
-      <c r="W35" s="8"/>
-      <c r="X35" s="8"/>
-      <c r="Y35" s="8">
-        <v>1</v>
-      </c>
-      <c r="Z35" s="8"/>
-      <c r="AA35" s="8"/>
-      <c r="AB35" s="8"/>
+      <c r="C35" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E35">
+        <v>1</v>
+      </c>
+      <c r="G35">
+        <v>1</v>
+      </c>
+      <c r="I35">
+        <v>1</v>
+      </c>
+      <c r="L35">
+        <v>1</v>
+      </c>
+      <c r="V35">
+        <v>1</v>
+      </c>
+      <c r="Y35">
+        <v>1</v>
+      </c>
     </row>
     <row r="36" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="A36" s="6" t="s">
+      <c r="A36" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B36" s="6" t="s">
+      <c r="B36" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C36" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D36" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E36" s="8">
-        <v>1</v>
-      </c>
-      <c r="F36" s="8"/>
-      <c r="G36" s="8">
-        <v>1</v>
-      </c>
-      <c r="H36" s="8">
-        <v>1</v>
-      </c>
-      <c r="I36" s="8"/>
-      <c r="J36" s="8"/>
-      <c r="K36" s="8">
-        <v>1</v>
-      </c>
-      <c r="L36" s="8"/>
-      <c r="M36" s="8"/>
-      <c r="N36" s="8"/>
-      <c r="O36" s="8"/>
-      <c r="P36" s="8"/>
-      <c r="Q36" s="8"/>
-      <c r="R36" s="8"/>
-      <c r="S36" s="8"/>
-      <c r="T36" s="8"/>
-      <c r="U36" s="8"/>
-      <c r="V36" s="8">
-        <v>1</v>
-      </c>
-      <c r="W36" s="8"/>
-      <c r="X36" s="8"/>
-      <c r="Y36" s="8">
-        <v>1</v>
-      </c>
-      <c r="Z36" s="8"/>
-      <c r="AA36" s="8"/>
-      <c r="AB36" s="8"/>
+      <c r="C36" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E36">
+        <v>1</v>
+      </c>
+      <c r="G36">
+        <v>1</v>
+      </c>
+      <c r="H36">
+        <v>1</v>
+      </c>
+      <c r="K36">
+        <v>1</v>
+      </c>
+      <c r="V36">
+        <v>1</v>
+      </c>
+      <c r="Y36">
+        <v>1</v>
+      </c>
     </row>
     <row r="37" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="A37" s="6" t="s">
+      <c r="A37" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B37" s="6" t="s">
+      <c r="B37" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C37" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D37" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E37" s="8">
-        <v>1</v>
-      </c>
-      <c r="F37" s="8"/>
-      <c r="G37" s="8">
-        <v>1</v>
-      </c>
-      <c r="H37" s="8">
-        <v>1</v>
-      </c>
-      <c r="I37" s="8">
-        <v>1</v>
-      </c>
-      <c r="J37" s="8"/>
-      <c r="K37" s="8">
-        <v>1</v>
-      </c>
-      <c r="L37" s="8">
-        <v>1</v>
-      </c>
-      <c r="M37" s="8"/>
-      <c r="N37" s="8"/>
-      <c r="O37" s="8"/>
-      <c r="P37" s="8"/>
-      <c r="Q37" s="8"/>
-      <c r="R37" s="8"/>
-      <c r="S37" s="8"/>
-      <c r="T37" s="8"/>
-      <c r="U37" s="8"/>
-      <c r="V37" s="8">
-        <v>1</v>
-      </c>
-      <c r="W37" s="8"/>
-      <c r="X37" s="8"/>
-      <c r="Y37" s="8">
-        <v>1</v>
-      </c>
-      <c r="Z37" s="8"/>
-      <c r="AA37" s="8"/>
-      <c r="AB37" s="8"/>
+      <c r="C37" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E37">
+        <v>1</v>
+      </c>
+      <c r="G37">
+        <v>1</v>
+      </c>
+      <c r="H37">
+        <v>1</v>
+      </c>
+      <c r="I37">
+        <v>1</v>
+      </c>
+      <c r="K37">
+        <v>1</v>
+      </c>
+      <c r="L37">
+        <v>1</v>
+      </c>
+      <c r="V37">
+        <v>1</v>
+      </c>
+      <c r="Y37">
+        <v>1</v>
+      </c>
     </row>
     <row r="38" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A38" s="1" t="s">
@@ -16740,7 +16659,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A81" s="1" t="s">
         <v>47</v>
       </c>
@@ -16781,7 +16700,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A82" s="1" t="s">
         <v>48</v>
       </c>
@@ -16810,7 +16729,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A83" s="1" t="s">
         <v>48</v>
       </c>
@@ -16845,7 +16764,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A84" s="1" t="s">
         <v>48</v>
       </c>
@@ -16880,7 +16799,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A85" s="1" t="s">
         <v>48</v>
       </c>
@@ -16921,7 +16840,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A86" s="1" t="s">
         <v>92</v>
       </c>
@@ -16947,7 +16866,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A87" s="1" t="s">
         <v>92</v>
       </c>
@@ -16979,7 +16898,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A88" s="1" t="s">
         <v>92</v>
       </c>
@@ -17011,7 +16930,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A89" s="1" t="s">
         <v>92</v>
       </c>
@@ -17049,423 +16968,287 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="A90" s="6" t="s">
+    <row r="90" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="A90" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B90" s="6" t="s">
+      <c r="B90" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C90" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D90" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E90" s="8"/>
-      <c r="F90" s="8"/>
-      <c r="G90" s="8">
-        <v>1</v>
-      </c>
-      <c r="H90" s="8"/>
-      <c r="I90" s="8"/>
-      <c r="J90" s="8"/>
-      <c r="K90" s="8"/>
-      <c r="L90" s="8"/>
-      <c r="M90" s="8"/>
-      <c r="N90" s="8"/>
-      <c r="O90" s="8"/>
-      <c r="P90" s="8">
-        <v>1</v>
-      </c>
-      <c r="Q90" s="8"/>
-      <c r="R90" s="8">
-        <v>1</v>
-      </c>
-      <c r="S90" s="8"/>
-      <c r="T90" s="8">
-        <v>1</v>
-      </c>
-      <c r="U90" s="8"/>
-      <c r="V90" s="8"/>
-      <c r="W90" s="8"/>
-      <c r="X90" s="8"/>
-      <c r="Y90" s="8">
-        <v>1</v>
-      </c>
-      <c r="Z90" s="8"/>
-      <c r="AA90" s="8"/>
-      <c r="AB90" s="8"/>
-    </row>
-    <row r="91" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="A91" s="6" t="s">
+      <c r="C90" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D90" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G90">
+        <v>1</v>
+      </c>
+      <c r="P90">
+        <v>1</v>
+      </c>
+      <c r="R90">
+        <v>1</v>
+      </c>
+      <c r="T90">
+        <v>1</v>
+      </c>
+      <c r="Y90">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="A91" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B91" s="6" t="s">
+      <c r="B91" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C91" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D91" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E91" s="8"/>
-      <c r="F91" s="8"/>
-      <c r="G91" s="8">
-        <v>1</v>
-      </c>
-      <c r="H91" s="8"/>
-      <c r="I91" s="8">
-        <v>1</v>
-      </c>
-      <c r="J91" s="8"/>
-      <c r="K91" s="8"/>
-      <c r="L91" s="8"/>
-      <c r="M91" s="8"/>
-      <c r="N91" s="8">
-        <v>1</v>
-      </c>
-      <c r="O91" s="8"/>
-      <c r="P91" s="8">
-        <v>1</v>
-      </c>
-      <c r="Q91" s="8"/>
-      <c r="R91" s="8">
-        <v>1</v>
-      </c>
-      <c r="S91" s="8"/>
-      <c r="T91" s="8">
-        <v>1</v>
-      </c>
-      <c r="U91" s="8"/>
-      <c r="V91" s="8"/>
-      <c r="W91" s="8"/>
-      <c r="X91" s="8"/>
-      <c r="Y91" s="8">
-        <v>1</v>
-      </c>
-      <c r="Z91" s="8"/>
-      <c r="AA91" s="8"/>
-      <c r="AB91" s="8"/>
-    </row>
-    <row r="92" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="A92" s="6" t="s">
+      <c r="C91" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D91" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G91">
+        <v>1</v>
+      </c>
+      <c r="I91">
+        <v>1</v>
+      </c>
+      <c r="N91">
+        <v>1</v>
+      </c>
+      <c r="P91">
+        <v>1</v>
+      </c>
+      <c r="R91">
+        <v>1</v>
+      </c>
+      <c r="T91">
+        <v>1</v>
+      </c>
+      <c r="Y91">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="A92" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B92" s="6" t="s">
+      <c r="B92" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C92" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D92" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E92" s="8"/>
-      <c r="F92" s="8"/>
-      <c r="G92" s="8">
-        <v>1</v>
-      </c>
-      <c r="H92" s="8">
-        <v>1</v>
-      </c>
-      <c r="I92" s="8"/>
-      <c r="J92" s="8"/>
-      <c r="K92" s="8"/>
-      <c r="L92" s="8"/>
-      <c r="M92" s="8">
-        <v>1</v>
-      </c>
-      <c r="N92" s="8"/>
-      <c r="O92" s="8"/>
-      <c r="P92" s="8">
-        <v>1</v>
-      </c>
-      <c r="Q92" s="8"/>
-      <c r="R92" s="8">
-        <v>1</v>
-      </c>
-      <c r="S92" s="8"/>
-      <c r="T92" s="8">
-        <v>1</v>
-      </c>
-      <c r="U92" s="8"/>
-      <c r="V92" s="8"/>
-      <c r="W92" s="8"/>
-      <c r="X92" s="8"/>
-      <c r="Y92" s="8">
-        <v>1</v>
-      </c>
-      <c r="Z92" s="8"/>
-      <c r="AA92" s="8"/>
-      <c r="AB92" s="8"/>
-    </row>
-    <row r="93" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="A93" s="6" t="s">
+      <c r="C92" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D92" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G92">
+        <v>1</v>
+      </c>
+      <c r="H92">
+        <v>1</v>
+      </c>
+      <c r="M92">
+        <v>1</v>
+      </c>
+      <c r="P92">
+        <v>1</v>
+      </c>
+      <c r="R92">
+        <v>1</v>
+      </c>
+      <c r="T92">
+        <v>1</v>
+      </c>
+      <c r="Y92">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="A93" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B93" s="6" t="s">
+      <c r="B93" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C93" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D93" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E93" s="8"/>
-      <c r="F93" s="8"/>
-      <c r="G93" s="8">
-        <v>1</v>
-      </c>
-      <c r="H93" s="8">
-        <v>1</v>
-      </c>
-      <c r="I93" s="8">
-        <v>1</v>
-      </c>
-      <c r="J93" s="8"/>
-      <c r="K93" s="8"/>
-      <c r="L93" s="8"/>
-      <c r="M93" s="8">
-        <v>1</v>
-      </c>
-      <c r="N93" s="8">
-        <v>1</v>
-      </c>
-      <c r="O93" s="8"/>
-      <c r="P93" s="8">
-        <v>1</v>
-      </c>
-      <c r="Q93" s="8"/>
-      <c r="R93" s="8">
-        <v>1</v>
-      </c>
-      <c r="S93" s="8"/>
-      <c r="T93" s="8">
-        <v>1</v>
-      </c>
-      <c r="U93" s="8"/>
-      <c r="V93" s="8"/>
-      <c r="W93" s="8"/>
-      <c r="X93" s="8"/>
-      <c r="Y93" s="8">
-        <v>1</v>
-      </c>
-      <c r="Z93" s="8"/>
-      <c r="AA93" s="8"/>
-      <c r="AB93" s="8"/>
-    </row>
-    <row r="94" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="A94" s="6" t="s">
+      <c r="C93" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D93" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G93">
+        <v>1</v>
+      </c>
+      <c r="H93">
+        <v>1</v>
+      </c>
+      <c r="I93">
+        <v>1</v>
+      </c>
+      <c r="M93">
+        <v>1</v>
+      </c>
+      <c r="N93">
+        <v>1</v>
+      </c>
+      <c r="P93">
+        <v>1</v>
+      </c>
+      <c r="R93">
+        <v>1</v>
+      </c>
+      <c r="T93">
+        <v>1</v>
+      </c>
+      <c r="Y93">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="A94" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B94" s="6" t="s">
+      <c r="B94" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C94" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D94" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E94" s="8"/>
-      <c r="F94" s="8"/>
-      <c r="G94" s="8">
-        <v>1</v>
-      </c>
-      <c r="H94" s="8"/>
-      <c r="I94" s="8"/>
-      <c r="J94" s="8"/>
-      <c r="K94" s="8"/>
-      <c r="L94" s="8"/>
-      <c r="M94" s="8"/>
-      <c r="N94" s="8"/>
-      <c r="O94" s="8"/>
-      <c r="P94" s="8">
-        <v>1</v>
-      </c>
-      <c r="Q94" s="8"/>
-      <c r="R94" s="8">
-        <v>1</v>
-      </c>
-      <c r="S94" s="8"/>
-      <c r="T94" s="8">
-        <v>1</v>
-      </c>
-      <c r="U94" s="8"/>
-      <c r="V94" s="8"/>
-      <c r="W94" s="8"/>
-      <c r="X94" s="8"/>
-      <c r="Y94" s="8">
-        <v>1</v>
-      </c>
-      <c r="Z94" s="8"/>
-      <c r="AA94" s="8"/>
-      <c r="AB94" s="8"/>
-    </row>
-    <row r="95" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="A95" s="6" t="s">
+      <c r="C94" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D94" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G94">
+        <v>1</v>
+      </c>
+      <c r="P94">
+        <v>1</v>
+      </c>
+      <c r="R94">
+        <v>1</v>
+      </c>
+      <c r="T94">
+        <v>1</v>
+      </c>
+      <c r="Y94">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="A95" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B95" s="6" t="s">
+      <c r="B95" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C95" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D95" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E95" s="8"/>
-      <c r="F95" s="8"/>
-      <c r="G95" s="8">
-        <v>1</v>
-      </c>
-      <c r="H95" s="8"/>
-      <c r="I95" s="8">
-        <v>1</v>
-      </c>
-      <c r="J95" s="8"/>
-      <c r="K95" s="8"/>
-      <c r="L95" s="8"/>
-      <c r="M95" s="8"/>
-      <c r="N95" s="8">
-        <v>1</v>
-      </c>
-      <c r="O95" s="8"/>
-      <c r="P95" s="8">
-        <v>1</v>
-      </c>
-      <c r="Q95" s="8"/>
-      <c r="R95" s="8">
-        <v>1</v>
-      </c>
-      <c r="S95" s="8"/>
-      <c r="T95" s="8">
-        <v>1</v>
-      </c>
-      <c r="U95" s="8"/>
-      <c r="V95" s="8"/>
-      <c r="W95" s="8"/>
-      <c r="X95" s="8"/>
-      <c r="Y95" s="8">
-        <v>1</v>
-      </c>
-      <c r="Z95" s="8"/>
-      <c r="AA95" s="8"/>
-      <c r="AB95" s="8"/>
-    </row>
-    <row r="96" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="A96" s="6" t="s">
+      <c r="C95" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D95" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G95">
+        <v>1</v>
+      </c>
+      <c r="I95">
+        <v>1</v>
+      </c>
+      <c r="N95">
+        <v>1</v>
+      </c>
+      <c r="P95">
+        <v>1</v>
+      </c>
+      <c r="R95">
+        <v>1</v>
+      </c>
+      <c r="T95">
+        <v>1</v>
+      </c>
+      <c r="Y95">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="A96" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B96" s="6" t="s">
+      <c r="B96" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C96" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D96" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E96" s="8"/>
-      <c r="F96" s="8"/>
-      <c r="G96" s="8">
-        <v>1</v>
-      </c>
-      <c r="H96" s="8">
-        <v>1</v>
-      </c>
-      <c r="I96" s="8"/>
-      <c r="J96" s="8"/>
-      <c r="K96" s="8"/>
-      <c r="L96" s="8"/>
-      <c r="M96" s="8">
-        <v>1</v>
-      </c>
-      <c r="N96" s="8"/>
-      <c r="O96" s="8"/>
-      <c r="P96" s="8">
-        <v>1</v>
-      </c>
-      <c r="Q96" s="8"/>
-      <c r="R96" s="8">
-        <v>1</v>
-      </c>
-      <c r="S96" s="8"/>
-      <c r="T96" s="8">
-        <v>1</v>
-      </c>
-      <c r="U96" s="8"/>
-      <c r="V96" s="8"/>
-      <c r="W96" s="8"/>
-      <c r="X96" s="8"/>
-      <c r="Y96" s="8">
-        <v>1</v>
-      </c>
-      <c r="Z96" s="8"/>
-      <c r="AA96" s="8"/>
-      <c r="AB96" s="8"/>
-    </row>
-    <row r="97" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="A97" s="6" t="s">
+      <c r="C96" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D96" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G96">
+        <v>1</v>
+      </c>
+      <c r="H96">
+        <v>1</v>
+      </c>
+      <c r="M96">
+        <v>1</v>
+      </c>
+      <c r="P96">
+        <v>1</v>
+      </c>
+      <c r="R96">
+        <v>1</v>
+      </c>
+      <c r="T96">
+        <v>1</v>
+      </c>
+      <c r="Y96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A97" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B97" s="6" t="s">
+      <c r="B97" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C97" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D97" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E97" s="8"/>
-      <c r="F97" s="8"/>
-      <c r="G97" s="8">
-        <v>1</v>
-      </c>
-      <c r="H97" s="8">
-        <v>1</v>
-      </c>
-      <c r="I97" s="8">
-        <v>1</v>
-      </c>
-      <c r="J97" s="8"/>
-      <c r="K97" s="8"/>
-      <c r="L97" s="8"/>
-      <c r="M97" s="8">
-        <v>1</v>
-      </c>
-      <c r="N97" s="8">
-        <v>1</v>
-      </c>
-      <c r="O97" s="8"/>
-      <c r="P97" s="8">
-        <v>1</v>
-      </c>
-      <c r="Q97" s="8"/>
-      <c r="R97" s="8">
-        <v>1</v>
-      </c>
-      <c r="S97" s="8"/>
-      <c r="T97" s="8">
-        <v>1</v>
-      </c>
-      <c r="U97" s="8"/>
-      <c r="V97" s="8"/>
-      <c r="W97" s="8"/>
-      <c r="X97" s="8"/>
-      <c r="Y97" s="8">
-        <v>1</v>
-      </c>
-      <c r="Z97" s="8"/>
-      <c r="AA97" s="8"/>
-      <c r="AB97" s="8"/>
-    </row>
-    <row r="98" spans="1:28" x14ac:dyDescent="0.45">
+      <c r="C97" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D97" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G97">
+        <v>1</v>
+      </c>
+      <c r="H97">
+        <v>1</v>
+      </c>
+      <c r="I97">
+        <v>1</v>
+      </c>
+      <c r="M97">
+        <v>1</v>
+      </c>
+      <c r="N97">
+        <v>1</v>
+      </c>
+      <c r="P97">
+        <v>1</v>
+      </c>
+      <c r="R97">
+        <v>1</v>
+      </c>
+      <c r="T97">
+        <v>1</v>
+      </c>
+      <c r="Y97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A98" s="1" t="s">
         <v>95</v>
       </c>
@@ -17488,7 +17271,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A99" s="1" t="s">
         <v>95</v>
       </c>
@@ -17517,7 +17300,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A100" s="1" t="s">
         <v>95</v>
       </c>
@@ -17546,7 +17329,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A101" s="1" t="s">
         <v>95</v>
       </c>
@@ -17581,7 +17364,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A102" s="1" t="s">
         <v>95</v>
       </c>
@@ -17607,7 +17390,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A103" s="1" t="s">
         <v>95</v>
       </c>
@@ -17639,7 +17422,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A104" s="1" t="s">
         <v>95</v>
       </c>
@@ -17671,7 +17454,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A105" s="1" t="s">
         <v>95</v>
       </c>
@@ -17709,7 +17492,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A106" s="1" t="s">
         <v>95</v>
       </c>
@@ -17735,7 +17518,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A107" s="1" t="s">
         <v>95</v>
       </c>
@@ -17767,7 +17550,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A108" s="1" t="s">
         <v>95</v>
       </c>
@@ -17799,7 +17582,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A109" s="1" t="s">
         <v>95</v>
       </c>
@@ -17837,7 +17620,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A110" s="1" t="s">
         <v>95</v>
       </c>
@@ -17866,7 +17649,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A111" s="1" t="s">
         <v>95</v>
       </c>
@@ -17901,7 +17684,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A112" s="1" t="s">
         <v>95</v>
       </c>
@@ -19469,7 +19252,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="161" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A161" s="1" t="s">
         <v>60</v>
       </c>
@@ -19501,463 +19284,307 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="A162" s="3" t="s">
+    <row r="162" spans="1:29" x14ac:dyDescent="0.45">
+      <c r="A162" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B162" s="3" t="s">
+      <c r="B162" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C162" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D162" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E162" s="5"/>
-      <c r="F162" s="5"/>
-      <c r="G162" s="5"/>
-      <c r="H162" s="5"/>
-      <c r="I162" s="5"/>
-      <c r="J162" s="5"/>
-      <c r="K162" s="5"/>
-      <c r="L162" s="5"/>
-      <c r="M162" s="5"/>
-      <c r="N162" s="5"/>
-      <c r="O162" s="5"/>
-      <c r="P162" s="5"/>
-      <c r="Q162" s="5"/>
-      <c r="R162" s="5"/>
-      <c r="S162" s="5"/>
-      <c r="T162" s="5"/>
-      <c r="U162" s="5"/>
-      <c r="V162" s="5"/>
-      <c r="W162" s="5"/>
-      <c r="X162" s="5"/>
-      <c r="Y162" s="5"/>
-      <c r="Z162" s="5"/>
-      <c r="AA162" s="5"/>
-      <c r="AB162" s="5"/>
-    </row>
-    <row r="163" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="A163" s="3" t="s">
+      <c r="C162" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D162" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y162">
+        <v>1</v>
+      </c>
+      <c r="AC162">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="163" spans="1:29" x14ac:dyDescent="0.45">
+      <c r="A163" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B163" s="3" t="s">
+      <c r="B163" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C163" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D163" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E163" s="5"/>
-      <c r="F163" s="5"/>
-      <c r="G163" s="5"/>
-      <c r="H163" s="5"/>
-      <c r="I163" s="5"/>
-      <c r="J163" s="5"/>
-      <c r="K163" s="5"/>
-      <c r="L163" s="5"/>
-      <c r="M163" s="5"/>
-      <c r="N163" s="5"/>
-      <c r="O163" s="5"/>
-      <c r="P163" s="5"/>
-      <c r="Q163" s="5"/>
-      <c r="R163" s="5"/>
-      <c r="S163" s="5"/>
-      <c r="T163" s="5"/>
-      <c r="U163" s="5"/>
-      <c r="V163" s="5"/>
-      <c r="W163" s="5"/>
-      <c r="X163" s="5"/>
-      <c r="Y163" s="5"/>
-      <c r="Z163" s="5"/>
-      <c r="AA163" s="5"/>
-      <c r="AB163" s="5"/>
-    </row>
-    <row r="164" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="A164" s="3" t="s">
+      <c r="C163" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D163" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="N163">
+        <v>1</v>
+      </c>
+      <c r="Y163">
+        <v>1</v>
+      </c>
+      <c r="AC163">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="164" spans="1:29" x14ac:dyDescent="0.45">
+      <c r="A164" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B164" s="3" t="s">
+      <c r="B164" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C164" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D164" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E164" s="5"/>
-      <c r="F164" s="5"/>
-      <c r="G164" s="5"/>
-      <c r="H164" s="5"/>
-      <c r="I164" s="5"/>
-      <c r="J164" s="5"/>
-      <c r="K164" s="5"/>
-      <c r="L164" s="5"/>
-      <c r="M164" s="5"/>
-      <c r="N164" s="5"/>
-      <c r="O164" s="5"/>
-      <c r="P164" s="5"/>
-      <c r="Q164" s="5"/>
-      <c r="R164" s="5"/>
-      <c r="S164" s="5"/>
-      <c r="T164" s="5"/>
-      <c r="U164" s="5"/>
-      <c r="V164" s="5"/>
-      <c r="W164" s="5"/>
-      <c r="X164" s="5"/>
-      <c r="Y164" s="5"/>
-      <c r="Z164" s="5"/>
-      <c r="AA164" s="5"/>
-      <c r="AB164" s="5"/>
-    </row>
-    <row r="165" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="A165" s="3" t="s">
+      <c r="C164" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D164" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M164">
+        <v>1</v>
+      </c>
+      <c r="Y164">
+        <v>1</v>
+      </c>
+      <c r="AC164">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="165" spans="1:29" x14ac:dyDescent="0.45">
+      <c r="A165" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B165" s="3" t="s">
+      <c r="B165" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C165" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D165" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E165" s="5"/>
-      <c r="F165" s="5"/>
-      <c r="G165" s="5"/>
-      <c r="H165" s="5"/>
-      <c r="I165" s="5"/>
-      <c r="J165" s="5"/>
-      <c r="K165" s="5"/>
-      <c r="L165" s="5"/>
-      <c r="M165" s="5"/>
-      <c r="N165" s="5"/>
-      <c r="O165" s="5"/>
-      <c r="P165" s="5"/>
-      <c r="Q165" s="5"/>
-      <c r="R165" s="5"/>
-      <c r="S165" s="5"/>
-      <c r="T165" s="5"/>
-      <c r="U165" s="5"/>
-      <c r="V165" s="5"/>
-      <c r="W165" s="5"/>
-      <c r="X165" s="5"/>
-      <c r="Y165" s="5"/>
-      <c r="Z165" s="5"/>
-      <c r="AA165" s="5"/>
-      <c r="AB165" s="5"/>
-    </row>
-    <row r="166" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="A166" s="3" t="s">
+      <c r="C165" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D165" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="M165">
+        <v>1</v>
+      </c>
+      <c r="N165">
+        <v>1</v>
+      </c>
+      <c r="Y165">
+        <v>1</v>
+      </c>
+      <c r="AC165">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="166" spans="1:29" x14ac:dyDescent="0.45">
+      <c r="A166" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B166" s="3" t="s">
+      <c r="B166" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C166" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D166" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E166" s="5"/>
-      <c r="F166" s="5"/>
-      <c r="G166" s="5"/>
-      <c r="H166" s="5"/>
-      <c r="I166" s="5"/>
-      <c r="J166" s="5"/>
-      <c r="K166" s="5"/>
-      <c r="L166" s="5"/>
-      <c r="M166" s="5"/>
-      <c r="N166" s="5"/>
-      <c r="O166" s="5"/>
-      <c r="P166" s="5"/>
-      <c r="Q166" s="5"/>
-      <c r="R166" s="5"/>
-      <c r="S166" s="5"/>
-      <c r="T166" s="5"/>
-      <c r="U166" s="5"/>
-      <c r="V166" s="5"/>
-      <c r="W166" s="5"/>
-      <c r="X166" s="5"/>
-      <c r="Y166" s="5"/>
-      <c r="Z166" s="5"/>
-      <c r="AA166" s="5"/>
-      <c r="AB166" s="5"/>
-    </row>
-    <row r="167" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="A167" s="3" t="s">
+      <c r="C166" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D166" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L166">
+        <v>1</v>
+      </c>
+      <c r="Y166">
+        <v>1</v>
+      </c>
+      <c r="AC166">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="167" spans="1:29" x14ac:dyDescent="0.45">
+      <c r="A167" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B167" s="3" t="s">
+      <c r="B167" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C167" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D167" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E167" s="5"/>
-      <c r="F167" s="5"/>
-      <c r="G167" s="5"/>
-      <c r="H167" s="5"/>
-      <c r="I167" s="5"/>
-      <c r="J167" s="5"/>
-      <c r="K167" s="5"/>
-      <c r="L167" s="5"/>
-      <c r="M167" s="5"/>
-      <c r="N167" s="5"/>
-      <c r="O167" s="5"/>
-      <c r="P167" s="5"/>
-      <c r="Q167" s="5"/>
-      <c r="R167" s="5"/>
-      <c r="S167" s="5"/>
-      <c r="T167" s="5"/>
-      <c r="U167" s="5"/>
-      <c r="V167" s="5"/>
-      <c r="W167" s="5"/>
-      <c r="X167" s="5"/>
-      <c r="Y167" s="5"/>
-      <c r="Z167" s="5"/>
-      <c r="AA167" s="5"/>
-      <c r="AB167" s="5"/>
-    </row>
-    <row r="168" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="A168" s="3" t="s">
+      <c r="C167" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D167" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L167">
+        <v>1</v>
+      </c>
+      <c r="N167">
+        <v>1</v>
+      </c>
+      <c r="Y167">
+        <v>1</v>
+      </c>
+      <c r="AC167">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="168" spans="1:29" x14ac:dyDescent="0.45">
+      <c r="A168" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B168" s="3" t="s">
+      <c r="B168" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C168" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D168" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E168" s="5"/>
-      <c r="F168" s="5"/>
-      <c r="G168" s="5"/>
-      <c r="H168" s="5"/>
-      <c r="I168" s="5"/>
-      <c r="J168" s="5"/>
-      <c r="K168" s="5"/>
-      <c r="L168" s="5"/>
-      <c r="M168" s="5"/>
-      <c r="N168" s="5"/>
-      <c r="O168" s="5"/>
-      <c r="P168" s="5"/>
-      <c r="Q168" s="5"/>
-      <c r="R168" s="5"/>
-      <c r="S168" s="5"/>
-      <c r="T168" s="5"/>
-      <c r="U168" s="5"/>
-      <c r="V168" s="5"/>
-      <c r="W168" s="5"/>
-      <c r="X168" s="5"/>
-      <c r="Y168" s="5"/>
-      <c r="Z168" s="5"/>
-      <c r="AA168" s="5"/>
-      <c r="AB168" s="5"/>
-    </row>
-    <row r="169" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="A169" s="3" t="s">
+      <c r="C168" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D168" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="L168">
+        <v>1</v>
+      </c>
+      <c r="M168">
+        <v>1</v>
+      </c>
+      <c r="Y168">
+        <v>1</v>
+      </c>
+      <c r="AC168">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="169" spans="1:29" x14ac:dyDescent="0.45">
+      <c r="A169" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B169" s="3" t="s">
+      <c r="B169" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C169" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D169" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E169" s="5"/>
-      <c r="F169" s="5"/>
-      <c r="G169" s="5"/>
-      <c r="H169" s="5"/>
-      <c r="I169" s="5"/>
-      <c r="J169" s="5"/>
-      <c r="K169" s="5"/>
-      <c r="L169" s="5"/>
-      <c r="M169" s="5"/>
-      <c r="N169" s="5"/>
-      <c r="O169" s="5"/>
-      <c r="P169" s="5"/>
-      <c r="Q169" s="5"/>
-      <c r="R169" s="5"/>
-      <c r="S169" s="5"/>
-      <c r="T169" s="5"/>
-      <c r="U169" s="5"/>
-      <c r="V169" s="5"/>
-      <c r="W169" s="5"/>
-      <c r="X169" s="5"/>
-      <c r="Y169" s="5"/>
-      <c r="Z169" s="5"/>
-      <c r="AA169" s="5"/>
-      <c r="AB169" s="5"/>
-    </row>
-    <row r="170" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="A170" s="3" t="s">
+      <c r="C169" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D169" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="L169">
+        <v>1</v>
+      </c>
+      <c r="M169">
+        <v>1</v>
+      </c>
+      <c r="N169">
+        <v>1</v>
+      </c>
+      <c r="Y169">
+        <v>1</v>
+      </c>
+      <c r="AC169">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="170" spans="1:29" x14ac:dyDescent="0.45">
+      <c r="A170" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B170" s="3" t="s">
+      <c r="B170" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C170" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D170" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E170" s="5"/>
-      <c r="F170" s="5"/>
-      <c r="G170" s="5"/>
-      <c r="H170" s="5"/>
-      <c r="I170" s="5"/>
-      <c r="J170" s="5"/>
-      <c r="K170" s="5"/>
-      <c r="L170" s="5"/>
-      <c r="M170" s="5"/>
-      <c r="N170" s="5"/>
-      <c r="O170" s="5"/>
-      <c r="P170" s="5"/>
-      <c r="Q170" s="5"/>
-      <c r="R170" s="5"/>
-      <c r="S170" s="5"/>
-      <c r="T170" s="5"/>
-      <c r="U170" s="5"/>
-      <c r="V170" s="5"/>
-      <c r="W170" s="5"/>
-      <c r="X170" s="5"/>
-      <c r="Y170" s="5"/>
-      <c r="Z170" s="5"/>
-      <c r="AA170" s="5"/>
-      <c r="AB170" s="5"/>
-    </row>
-    <row r="171" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="A171" s="3" t="s">
+      <c r="C170" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D170" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K170">
+        <v>1</v>
+      </c>
+      <c r="Y170">
+        <v>1</v>
+      </c>
+      <c r="AC170">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="171" spans="1:29" x14ac:dyDescent="0.45">
+      <c r="A171" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B171" s="3" t="s">
+      <c r="B171" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C171" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D171" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E171" s="5"/>
-      <c r="F171" s="5"/>
-      <c r="G171" s="5"/>
-      <c r="H171" s="5"/>
-      <c r="I171" s="5"/>
-      <c r="J171" s="5"/>
-      <c r="K171" s="5"/>
-      <c r="L171" s="5"/>
-      <c r="M171" s="5"/>
-      <c r="N171" s="5"/>
-      <c r="O171" s="5"/>
-      <c r="P171" s="5"/>
-      <c r="Q171" s="5"/>
-      <c r="R171" s="5"/>
-      <c r="S171" s="5"/>
-      <c r="T171" s="5"/>
-      <c r="U171" s="5"/>
-      <c r="V171" s="5"/>
-      <c r="W171" s="5"/>
-      <c r="X171" s="5"/>
-      <c r="Y171" s="5"/>
-      <c r="Z171" s="5"/>
-      <c r="AA171" s="5"/>
-      <c r="AB171" s="5"/>
-    </row>
-    <row r="172" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="A172" s="3" t="s">
+      <c r="C171" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D171" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K171">
+        <v>1</v>
+      </c>
+      <c r="N171">
+        <v>1</v>
+      </c>
+      <c r="Y171">
+        <v>1</v>
+      </c>
+      <c r="AC171">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="172" spans="1:29" x14ac:dyDescent="0.45">
+      <c r="A172" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B172" s="3" t="s">
+      <c r="B172" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C172" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D172" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E172" s="5"/>
-      <c r="F172" s="5"/>
-      <c r="G172" s="5"/>
-      <c r="H172" s="5"/>
-      <c r="I172" s="5"/>
-      <c r="J172" s="5"/>
-      <c r="K172" s="5"/>
-      <c r="L172" s="5"/>
-      <c r="M172" s="5"/>
-      <c r="N172" s="5"/>
-      <c r="O172" s="5"/>
-      <c r="P172" s="5"/>
-      <c r="Q172" s="5"/>
-      <c r="R172" s="5"/>
-      <c r="S172" s="5"/>
-      <c r="T172" s="5"/>
-      <c r="U172" s="5"/>
-      <c r="V172" s="5"/>
-      <c r="W172" s="5"/>
-      <c r="X172" s="5"/>
-      <c r="Y172" s="5"/>
-      <c r="Z172" s="5"/>
-      <c r="AA172" s="5"/>
-      <c r="AB172" s="5"/>
-    </row>
-    <row r="173" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="A173" s="3" t="s">
+      <c r="C172" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D172" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K172">
+        <v>1</v>
+      </c>
+      <c r="M172">
+        <v>1</v>
+      </c>
+      <c r="Y172">
+        <v>1</v>
+      </c>
+      <c r="AC172">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="173" spans="1:29" x14ac:dyDescent="0.45">
+      <c r="A173" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B173" s="3" t="s">
+      <c r="B173" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C173" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D173" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E173" s="5"/>
-      <c r="F173" s="5"/>
-      <c r="G173" s="5"/>
-      <c r="H173" s="5"/>
-      <c r="I173" s="5"/>
-      <c r="J173" s="5"/>
-      <c r="K173" s="5"/>
-      <c r="L173" s="5"/>
-      <c r="M173" s="5"/>
-      <c r="N173" s="5"/>
-      <c r="O173" s="5"/>
-      <c r="P173" s="5"/>
-      <c r="Q173" s="5"/>
-      <c r="R173" s="5"/>
-      <c r="S173" s="5"/>
-      <c r="T173" s="5"/>
-      <c r="U173" s="5"/>
-      <c r="V173" s="5"/>
-      <c r="W173" s="5"/>
-      <c r="X173" s="5"/>
-      <c r="Y173" s="5"/>
-      <c r="Z173" s="5"/>
-      <c r="AA173" s="5"/>
-      <c r="AB173" s="5"/>
-    </row>
-    <row r="174" spans="1:28" x14ac:dyDescent="0.45">
+      <c r="C173" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D173" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K173">
+        <v>1</v>
+      </c>
+      <c r="M173">
+        <v>1</v>
+      </c>
+      <c r="N173">
+        <v>1</v>
+      </c>
+      <c r="Y173">
+        <v>1</v>
+      </c>
+      <c r="AC173">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="174" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A174" s="1" t="s">
         <v>61</v>
       </c>
@@ -19977,7 +19604,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="175" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="175" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A175" s="1" t="s">
         <v>61</v>
       </c>
@@ -19997,7 +19624,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="176" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="176" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A176" s="1" t="s">
         <v>61</v>
       </c>
@@ -22011,7 +21638,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="241" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="241" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A241" s="1" t="s">
         <v>80</v>
       </c>
@@ -22052,836 +21679,568 @@
         <v>1</v>
       </c>
     </row>
-    <row r="242" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="A242" s="6" t="s">
+    <row r="242" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="A242" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B242" s="6" t="s">
+      <c r="B242" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C242" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D242" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E242" s="8"/>
-      <c r="F242" s="8"/>
-      <c r="G242" s="8">
-        <v>1</v>
-      </c>
-      <c r="H242" s="8"/>
-      <c r="I242" s="8"/>
-      <c r="J242" s="8"/>
-      <c r="K242" s="8"/>
-      <c r="L242" s="8"/>
-      <c r="M242" s="8"/>
-      <c r="N242" s="8"/>
-      <c r="O242" s="8"/>
-      <c r="P242" s="8">
-        <v>1</v>
-      </c>
-      <c r="Q242" s="8"/>
-      <c r="R242" s="8"/>
-      <c r="S242" s="8"/>
-      <c r="T242" s="8"/>
-      <c r="U242" s="8"/>
-      <c r="V242" s="8"/>
-      <c r="W242" s="8"/>
-      <c r="X242" s="8"/>
-      <c r="Y242" s="8">
-        <v>1</v>
-      </c>
-      <c r="Z242" s="8"/>
-      <c r="AA242" s="8"/>
-      <c r="AB242" s="8"/>
-    </row>
-    <row r="243" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="A243" s="6" t="s">
+      <c r="C242" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D242" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G242">
+        <v>1</v>
+      </c>
+      <c r="P242">
+        <v>1</v>
+      </c>
+      <c r="Y242">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="243" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="A243" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B243" s="6" t="s">
+      <c r="B243" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C243" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D243" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E243" s="8"/>
-      <c r="F243" s="8"/>
-      <c r="G243" s="8">
-        <v>1</v>
-      </c>
-      <c r="H243" s="8"/>
-      <c r="I243" s="8">
-        <v>1</v>
-      </c>
-      <c r="J243" s="8"/>
-      <c r="K243" s="8"/>
-      <c r="L243" s="8"/>
-      <c r="M243" s="8"/>
-      <c r="N243" s="8">
-        <v>1</v>
-      </c>
-      <c r="O243" s="8"/>
-      <c r="P243" s="8">
-        <v>1</v>
-      </c>
-      <c r="Q243" s="8"/>
-      <c r="R243" s="8"/>
-      <c r="S243" s="8"/>
-      <c r="T243" s="8"/>
-      <c r="U243" s="8"/>
-      <c r="V243" s="8"/>
-      <c r="W243" s="8"/>
-      <c r="X243" s="8"/>
-      <c r="Y243" s="8">
-        <v>1</v>
-      </c>
-      <c r="Z243" s="8"/>
-      <c r="AA243" s="8"/>
-      <c r="AB243" s="8"/>
-    </row>
-    <row r="244" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="A244" s="6" t="s">
+      <c r="C243" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D243" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G243">
+        <v>1</v>
+      </c>
+      <c r="I243">
+        <v>1</v>
+      </c>
+      <c r="N243">
+        <v>1</v>
+      </c>
+      <c r="P243">
+        <v>1</v>
+      </c>
+      <c r="Y243">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="244" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="A244" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B244" s="6" t="s">
+      <c r="B244" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C244" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D244" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E244" s="8"/>
-      <c r="F244" s="8"/>
-      <c r="G244" s="8">
-        <v>1</v>
-      </c>
-      <c r="H244" s="8">
-        <v>1</v>
-      </c>
-      <c r="I244" s="8"/>
-      <c r="J244" s="8"/>
-      <c r="K244" s="8"/>
-      <c r="L244" s="8"/>
-      <c r="M244" s="8">
-        <v>1</v>
-      </c>
-      <c r="N244" s="8"/>
-      <c r="O244" s="8"/>
-      <c r="P244" s="8">
-        <v>1</v>
-      </c>
-      <c r="Q244" s="8"/>
-      <c r="R244" s="8"/>
-      <c r="S244" s="8"/>
-      <c r="T244" s="8"/>
-      <c r="U244" s="8"/>
-      <c r="V244" s="8"/>
-      <c r="W244" s="8"/>
-      <c r="X244" s="8"/>
-      <c r="Y244" s="8">
-        <v>1</v>
-      </c>
-      <c r="Z244" s="8"/>
-      <c r="AA244" s="8"/>
-      <c r="AB244" s="8"/>
-    </row>
-    <row r="245" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="A245" s="6" t="s">
+      <c r="C244" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D244" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G244">
+        <v>1</v>
+      </c>
+      <c r="H244">
+        <v>1</v>
+      </c>
+      <c r="M244">
+        <v>1</v>
+      </c>
+      <c r="P244">
+        <v>1</v>
+      </c>
+      <c r="Y244">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="245" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="A245" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B245" s="6" t="s">
+      <c r="B245" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C245" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D245" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E245" s="8"/>
-      <c r="F245" s="8"/>
-      <c r="G245" s="8">
-        <v>1</v>
-      </c>
-      <c r="H245" s="8">
-        <v>1</v>
-      </c>
-      <c r="I245" s="8">
-        <v>1</v>
-      </c>
-      <c r="J245" s="8"/>
-      <c r="K245" s="8"/>
-      <c r="L245" s="8"/>
-      <c r="M245" s="8">
-        <v>1</v>
-      </c>
-      <c r="N245" s="8">
-        <v>1</v>
-      </c>
-      <c r="O245" s="8"/>
-      <c r="P245" s="8">
-        <v>1</v>
-      </c>
-      <c r="Q245" s="8"/>
-      <c r="R245" s="8"/>
-      <c r="S245" s="8"/>
-      <c r="T245" s="8"/>
-      <c r="U245" s="8"/>
-      <c r="V245" s="8"/>
-      <c r="W245" s="8"/>
-      <c r="X245" s="8"/>
-      <c r="Y245" s="8">
-        <v>1</v>
-      </c>
-      <c r="Z245" s="8"/>
-      <c r="AA245" s="8"/>
-      <c r="AB245" s="8"/>
-    </row>
-    <row r="246" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="A246" s="6" t="s">
+      <c r="C245" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D245" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G245">
+        <v>1</v>
+      </c>
+      <c r="H245">
+        <v>1</v>
+      </c>
+      <c r="I245">
+        <v>1</v>
+      </c>
+      <c r="M245">
+        <v>1</v>
+      </c>
+      <c r="N245">
+        <v>1</v>
+      </c>
+      <c r="P245">
+        <v>1</v>
+      </c>
+      <c r="Y245">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="246" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="A246" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B246" s="6" t="s">
+      <c r="B246" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C246" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D246" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E246" s="8"/>
-      <c r="F246" s="8"/>
-      <c r="G246" s="8">
-        <v>1</v>
-      </c>
-      <c r="H246" s="8"/>
-      <c r="I246" s="8"/>
-      <c r="J246" s="8"/>
-      <c r="K246" s="8"/>
-      <c r="L246" s="8"/>
-      <c r="M246" s="8"/>
-      <c r="N246" s="8"/>
-      <c r="O246" s="8"/>
-      <c r="P246" s="8">
-        <v>1</v>
-      </c>
-      <c r="Q246" s="8">
-        <v>1</v>
-      </c>
-      <c r="S246" s="8"/>
-      <c r="T246" s="8">
-        <v>1</v>
-      </c>
-      <c r="U246" s="8"/>
-      <c r="V246" s="8"/>
-      <c r="W246" s="8"/>
-      <c r="X246" s="8"/>
-      <c r="Y246" s="8">
-        <v>1</v>
-      </c>
-      <c r="Z246" s="8"/>
-      <c r="AA246" s="8"/>
-      <c r="AB246" s="8"/>
-    </row>
-    <row r="247" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="A247" s="6" t="s">
+      <c r="C246" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D246" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G246">
+        <v>1</v>
+      </c>
+      <c r="P246">
+        <v>1</v>
+      </c>
+      <c r="Q246">
+        <v>1</v>
+      </c>
+      <c r="T246">
+        <v>1</v>
+      </c>
+      <c r="Y246">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="247" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="A247" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B247" s="6" t="s">
+      <c r="B247" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C247" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D247" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E247" s="8"/>
-      <c r="F247" s="8"/>
-      <c r="G247" s="8">
-        <v>1</v>
-      </c>
-      <c r="H247" s="8"/>
-      <c r="I247" s="8">
-        <v>1</v>
-      </c>
-      <c r="J247" s="8"/>
-      <c r="K247" s="8"/>
-      <c r="L247" s="8"/>
-      <c r="M247" s="8"/>
-      <c r="N247" s="8">
-        <v>1</v>
-      </c>
-      <c r="O247" s="8"/>
-      <c r="P247" s="8">
-        <v>1</v>
-      </c>
-      <c r="Q247" s="8">
-        <v>1</v>
-      </c>
-      <c r="S247" s="8"/>
-      <c r="T247" s="8">
-        <v>1</v>
-      </c>
-      <c r="U247" s="8"/>
-      <c r="V247" s="8"/>
-      <c r="W247" s="8"/>
-      <c r="X247" s="8"/>
-      <c r="Y247" s="8">
-        <v>1</v>
-      </c>
-      <c r="Z247" s="8"/>
-      <c r="AA247" s="8"/>
-      <c r="AB247" s="8"/>
-    </row>
-    <row r="248" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="A248" s="6" t="s">
+      <c r="C247" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D247" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G247">
+        <v>1</v>
+      </c>
+      <c r="I247">
+        <v>1</v>
+      </c>
+      <c r="N247">
+        <v>1</v>
+      </c>
+      <c r="P247">
+        <v>1</v>
+      </c>
+      <c r="Q247">
+        <v>1</v>
+      </c>
+      <c r="T247">
+        <v>1</v>
+      </c>
+      <c r="Y247">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="248" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="A248" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B248" s="6" t="s">
+      <c r="B248" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C248" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D248" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E248" s="8"/>
-      <c r="F248" s="8"/>
-      <c r="G248" s="8">
-        <v>1</v>
-      </c>
-      <c r="H248" s="8">
-        <v>1</v>
-      </c>
-      <c r="I248" s="8"/>
-      <c r="J248" s="8"/>
-      <c r="K248" s="8"/>
-      <c r="L248" s="8"/>
-      <c r="M248" s="8">
-        <v>1</v>
-      </c>
-      <c r="N248" s="8"/>
-      <c r="O248" s="8"/>
-      <c r="P248" s="8">
-        <v>1</v>
-      </c>
-      <c r="Q248" s="8">
-        <v>1</v>
-      </c>
-      <c r="S248" s="8"/>
-      <c r="T248" s="8">
-        <v>1</v>
-      </c>
-      <c r="U248" s="8"/>
-      <c r="V248" s="8"/>
-      <c r="W248" s="8"/>
-      <c r="X248" s="8"/>
-      <c r="Y248" s="8">
-        <v>1</v>
-      </c>
-      <c r="Z248" s="8"/>
-      <c r="AA248" s="8"/>
-      <c r="AB248" s="8"/>
-    </row>
-    <row r="249" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="A249" s="6" t="s">
+      <c r="C248" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D248" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G248">
+        <v>1</v>
+      </c>
+      <c r="H248">
+        <v>1</v>
+      </c>
+      <c r="M248">
+        <v>1</v>
+      </c>
+      <c r="P248">
+        <v>1</v>
+      </c>
+      <c r="Q248">
+        <v>1</v>
+      </c>
+      <c r="T248">
+        <v>1</v>
+      </c>
+      <c r="Y248">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="249" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="A249" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B249" s="6" t="s">
+      <c r="B249" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C249" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D249" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E249" s="8"/>
-      <c r="F249" s="8"/>
-      <c r="G249" s="8">
-        <v>1</v>
-      </c>
-      <c r="H249" s="8">
-        <v>1</v>
-      </c>
-      <c r="I249" s="8">
-        <v>1</v>
-      </c>
-      <c r="J249" s="8"/>
-      <c r="K249" s="8"/>
-      <c r="L249" s="8"/>
-      <c r="M249" s="8">
-        <v>1</v>
-      </c>
-      <c r="N249" s="8">
-        <v>1</v>
-      </c>
-      <c r="O249" s="8"/>
-      <c r="P249" s="8">
-        <v>1</v>
-      </c>
-      <c r="Q249" s="8">
-        <v>1</v>
-      </c>
-      <c r="S249" s="8"/>
-      <c r="T249" s="8">
-        <v>1</v>
-      </c>
-      <c r="U249" s="8"/>
-      <c r="V249" s="8"/>
-      <c r="W249" s="8"/>
-      <c r="X249" s="8"/>
-      <c r="Y249" s="8">
-        <v>1</v>
-      </c>
-      <c r="Z249" s="8"/>
-      <c r="AA249" s="8"/>
-      <c r="AB249" s="8"/>
-    </row>
-    <row r="250" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="A250" s="6" t="s">
+      <c r="C249" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D249" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G249">
+        <v>1</v>
+      </c>
+      <c r="H249">
+        <v>1</v>
+      </c>
+      <c r="I249">
+        <v>1</v>
+      </c>
+      <c r="M249">
+        <v>1</v>
+      </c>
+      <c r="N249">
+        <v>1</v>
+      </c>
+      <c r="P249">
+        <v>1</v>
+      </c>
+      <c r="Q249">
+        <v>1</v>
+      </c>
+      <c r="T249">
+        <v>1</v>
+      </c>
+      <c r="Y249">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="250" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="A250" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B250" s="6" t="s">
+      <c r="B250" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C250" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D250" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E250" s="8"/>
-      <c r="F250" s="8"/>
-      <c r="G250" s="8">
-        <v>1</v>
-      </c>
-      <c r="H250" s="8"/>
-      <c r="I250" s="8"/>
-      <c r="J250" s="8"/>
-      <c r="K250" s="8"/>
-      <c r="L250" s="8"/>
-      <c r="M250" s="8"/>
-      <c r="N250" s="8"/>
-      <c r="O250" s="8"/>
-      <c r="P250" s="8">
-        <v>1</v>
-      </c>
-      <c r="Q250" s="8">
-        <v>1</v>
-      </c>
-      <c r="R250" s="8">
-        <v>1</v>
-      </c>
-      <c r="S250" s="8"/>
-      <c r="T250" s="8">
-        <v>1</v>
-      </c>
-      <c r="U250" s="8"/>
-      <c r="V250" s="8"/>
-      <c r="W250" s="8"/>
-      <c r="X250" s="8"/>
-      <c r="Y250" s="8">
-        <v>1</v>
-      </c>
-      <c r="Z250" s="8"/>
-      <c r="AA250" s="8"/>
-      <c r="AB250" s="8"/>
-    </row>
-    <row r="251" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="A251" s="6" t="s">
+      <c r="C250" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D250" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G250">
+        <v>1</v>
+      </c>
+      <c r="P250">
+        <v>1</v>
+      </c>
+      <c r="Q250">
+        <v>1</v>
+      </c>
+      <c r="R250">
+        <v>1</v>
+      </c>
+      <c r="T250">
+        <v>1</v>
+      </c>
+      <c r="Y250">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="251" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="A251" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B251" s="6" t="s">
+      <c r="B251" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C251" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D251" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E251" s="8"/>
-      <c r="F251" s="8"/>
-      <c r="G251" s="8">
-        <v>1</v>
-      </c>
-      <c r="H251" s="8"/>
-      <c r="I251" s="8">
-        <v>1</v>
-      </c>
-      <c r="J251" s="8"/>
-      <c r="K251" s="8"/>
-      <c r="L251" s="8"/>
-      <c r="M251" s="8"/>
-      <c r="N251" s="8">
-        <v>1</v>
-      </c>
-      <c r="O251" s="8"/>
-      <c r="P251" s="8">
-        <v>1</v>
-      </c>
-      <c r="Q251" s="8">
-        <v>1</v>
-      </c>
-      <c r="R251" s="8">
-        <v>1</v>
-      </c>
-      <c r="S251" s="8"/>
-      <c r="T251" s="8">
-        <v>1</v>
-      </c>
-      <c r="U251" s="8"/>
-      <c r="V251" s="8"/>
-      <c r="W251" s="8"/>
-      <c r="X251" s="8"/>
-      <c r="Y251" s="8">
-        <v>1</v>
-      </c>
-      <c r="Z251" s="8"/>
-      <c r="AA251" s="8"/>
-      <c r="AB251" s="8"/>
-    </row>
-    <row r="252" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="A252" s="6" t="s">
+      <c r="C251" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D251" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G251">
+        <v>1</v>
+      </c>
+      <c r="I251">
+        <v>1</v>
+      </c>
+      <c r="N251">
+        <v>1</v>
+      </c>
+      <c r="P251">
+        <v>1</v>
+      </c>
+      <c r="Q251">
+        <v>1</v>
+      </c>
+      <c r="R251">
+        <v>1</v>
+      </c>
+      <c r="T251">
+        <v>1</v>
+      </c>
+      <c r="Y251">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="252" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="A252" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B252" s="6" t="s">
+      <c r="B252" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C252" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D252" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E252" s="8"/>
-      <c r="F252" s="8"/>
-      <c r="G252" s="8">
-        <v>1</v>
-      </c>
-      <c r="H252" s="8">
-        <v>1</v>
-      </c>
-      <c r="I252" s="8"/>
-      <c r="J252" s="8"/>
-      <c r="K252" s="8"/>
-      <c r="L252" s="8"/>
-      <c r="M252" s="8">
-        <v>1</v>
-      </c>
-      <c r="N252" s="8"/>
-      <c r="O252" s="8"/>
-      <c r="P252" s="8">
-        <v>1</v>
-      </c>
-      <c r="Q252" s="8">
-        <v>1</v>
-      </c>
-      <c r="R252" s="8">
-        <v>1</v>
-      </c>
-      <c r="S252" s="8"/>
-      <c r="T252" s="8">
-        <v>1</v>
-      </c>
-      <c r="U252" s="8"/>
-      <c r="V252" s="8"/>
-      <c r="W252" s="8"/>
-      <c r="X252" s="8"/>
-      <c r="Y252" s="8">
-        <v>1</v>
-      </c>
-      <c r="Z252" s="8"/>
-      <c r="AA252" s="8"/>
-      <c r="AB252" s="8"/>
-    </row>
-    <row r="253" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="A253" s="6" t="s">
+      <c r="C252" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D252" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G252">
+        <v>1</v>
+      </c>
+      <c r="H252">
+        <v>1</v>
+      </c>
+      <c r="M252">
+        <v>1</v>
+      </c>
+      <c r="P252">
+        <v>1</v>
+      </c>
+      <c r="Q252">
+        <v>1</v>
+      </c>
+      <c r="R252">
+        <v>1</v>
+      </c>
+      <c r="T252">
+        <v>1</v>
+      </c>
+      <c r="Y252">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="253" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="A253" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B253" s="6" t="s">
+      <c r="B253" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C253" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D253" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E253" s="8"/>
-      <c r="F253" s="8"/>
-      <c r="G253" s="8">
-        <v>1</v>
-      </c>
-      <c r="H253" s="8">
-        <v>1</v>
-      </c>
-      <c r="I253" s="8">
-        <v>1</v>
-      </c>
-      <c r="J253" s="8"/>
-      <c r="K253" s="8"/>
-      <c r="L253" s="8"/>
-      <c r="M253" s="8">
-        <v>1</v>
-      </c>
-      <c r="N253" s="8">
-        <v>1</v>
-      </c>
-      <c r="O253" s="8"/>
-      <c r="P253" s="8">
-        <v>1</v>
-      </c>
-      <c r="Q253" s="8">
-        <v>1</v>
-      </c>
-      <c r="R253" s="8">
-        <v>1</v>
-      </c>
-      <c r="S253" s="8"/>
-      <c r="T253" s="8">
-        <v>1</v>
-      </c>
-      <c r="U253" s="8"/>
-      <c r="V253" s="8"/>
-      <c r="W253" s="8"/>
-      <c r="X253" s="8"/>
-      <c r="Y253" s="8">
-        <v>1</v>
-      </c>
-      <c r="Z253" s="8"/>
-      <c r="AA253" s="8"/>
-      <c r="AB253" s="8"/>
-    </row>
-    <row r="254" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="A254" s="6" t="s">
+      <c r="C253" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D253" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G253">
+        <v>1</v>
+      </c>
+      <c r="H253">
+        <v>1</v>
+      </c>
+      <c r="I253">
+        <v>1</v>
+      </c>
+      <c r="M253">
+        <v>1</v>
+      </c>
+      <c r="N253">
+        <v>1</v>
+      </c>
+      <c r="P253">
+        <v>1</v>
+      </c>
+      <c r="Q253">
+        <v>1</v>
+      </c>
+      <c r="R253">
+        <v>1</v>
+      </c>
+      <c r="T253">
+        <v>1</v>
+      </c>
+      <c r="Y253">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="254" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="A254" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B254" s="6" t="s">
+      <c r="B254" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C254" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D254" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E254" s="8"/>
-      <c r="F254" s="8"/>
-      <c r="G254" s="8">
-        <v>1</v>
-      </c>
-      <c r="H254" s="8"/>
-      <c r="I254" s="8"/>
-      <c r="J254" s="8"/>
-      <c r="K254" s="8"/>
-      <c r="L254" s="8"/>
-      <c r="M254" s="8"/>
-      <c r="N254" s="8"/>
-      <c r="O254" s="8"/>
-      <c r="P254" s="8">
-        <v>1</v>
-      </c>
-      <c r="Q254" s="8">
-        <v>1</v>
-      </c>
-      <c r="R254" s="8">
-        <v>1</v>
-      </c>
-      <c r="S254" s="8"/>
-      <c r="T254" s="8">
-        <v>1</v>
-      </c>
-      <c r="U254" s="8"/>
-      <c r="V254" s="8"/>
-      <c r="W254" s="8"/>
-      <c r="X254" s="8"/>
-      <c r="Y254" s="8">
-        <v>1</v>
-      </c>
-      <c r="Z254" s="8"/>
-      <c r="AA254" s="8"/>
-      <c r="AB254" s="8"/>
-    </row>
-    <row r="255" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="A255" s="6" t="s">
+      <c r="C254" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D254" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G254">
+        <v>1</v>
+      </c>
+      <c r="P254">
+        <v>1</v>
+      </c>
+      <c r="Q254">
+        <v>1</v>
+      </c>
+      <c r="R254">
+        <v>1</v>
+      </c>
+      <c r="T254">
+        <v>1</v>
+      </c>
+      <c r="Y254">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="255" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="A255" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B255" s="6" t="s">
+      <c r="B255" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C255" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D255" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E255" s="8"/>
-      <c r="F255" s="8"/>
-      <c r="G255" s="8">
-        <v>1</v>
-      </c>
-      <c r="H255" s="8"/>
-      <c r="I255" s="8">
-        <v>1</v>
-      </c>
-      <c r="J255" s="8"/>
-      <c r="K255" s="8"/>
-      <c r="L255" s="8"/>
-      <c r="M255" s="8"/>
-      <c r="N255" s="8">
-        <v>1</v>
-      </c>
-      <c r="O255" s="8"/>
-      <c r="P255" s="8">
-        <v>1</v>
-      </c>
-      <c r="Q255" s="8">
-        <v>1</v>
-      </c>
-      <c r="R255" s="8">
-        <v>1</v>
-      </c>
-      <c r="S255" s="8"/>
-      <c r="T255" s="8">
-        <v>1</v>
-      </c>
-      <c r="U255" s="8"/>
-      <c r="V255" s="8"/>
-      <c r="W255" s="8"/>
-      <c r="X255" s="8"/>
-      <c r="Y255" s="8">
-        <v>1</v>
-      </c>
-      <c r="Z255" s="8"/>
-      <c r="AA255" s="8"/>
-      <c r="AB255" s="8"/>
-    </row>
-    <row r="256" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="A256" s="6" t="s">
+      <c r="C255" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D255" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G255">
+        <v>1</v>
+      </c>
+      <c r="I255">
+        <v>1</v>
+      </c>
+      <c r="N255">
+        <v>1</v>
+      </c>
+      <c r="P255">
+        <v>1</v>
+      </c>
+      <c r="Q255">
+        <v>1</v>
+      </c>
+      <c r="R255">
+        <v>1</v>
+      </c>
+      <c r="T255">
+        <v>1</v>
+      </c>
+      <c r="Y255">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="256" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="A256" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B256" s="6" t="s">
+      <c r="B256" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C256" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D256" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E256" s="8"/>
-      <c r="F256" s="8"/>
-      <c r="G256" s="8">
-        <v>1</v>
-      </c>
-      <c r="H256" s="8">
-        <v>1</v>
-      </c>
-      <c r="I256" s="8"/>
-      <c r="J256" s="8"/>
-      <c r="K256" s="8"/>
-      <c r="L256" s="8"/>
-      <c r="M256" s="8">
-        <v>1</v>
-      </c>
-      <c r="N256" s="8"/>
-      <c r="O256" s="8"/>
-      <c r="P256" s="8">
-        <v>1</v>
-      </c>
-      <c r="Q256" s="8">
-        <v>1</v>
-      </c>
-      <c r="R256" s="8">
-        <v>1</v>
-      </c>
-      <c r="S256" s="8"/>
-      <c r="T256" s="8">
-        <v>1</v>
-      </c>
-      <c r="U256" s="8"/>
-      <c r="V256" s="8"/>
-      <c r="W256" s="8"/>
-      <c r="X256" s="8"/>
-      <c r="Y256" s="8">
-        <v>1</v>
-      </c>
-      <c r="Z256" s="8"/>
-      <c r="AA256" s="8"/>
-      <c r="AB256" s="8"/>
-    </row>
-    <row r="257" spans="1:28" x14ac:dyDescent="0.45">
-      <c r="A257" s="6" t="s">
+      <c r="C256" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D256" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G256">
+        <v>1</v>
+      </c>
+      <c r="H256">
+        <v>1</v>
+      </c>
+      <c r="M256">
+        <v>1</v>
+      </c>
+      <c r="P256">
+        <v>1</v>
+      </c>
+      <c r="Q256">
+        <v>1</v>
+      </c>
+      <c r="R256">
+        <v>1</v>
+      </c>
+      <c r="T256">
+        <v>1</v>
+      </c>
+      <c r="Y256">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="257" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A257" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B257" s="6" t="s">
+      <c r="B257" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C257" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D257" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E257" s="8"/>
-      <c r="F257" s="8"/>
-      <c r="G257" s="8">
-        <v>1</v>
-      </c>
-      <c r="H257" s="8">
-        <v>1</v>
-      </c>
-      <c r="I257" s="8">
-        <v>1</v>
-      </c>
-      <c r="J257" s="8"/>
-      <c r="K257" s="8"/>
-      <c r="L257" s="8"/>
-      <c r="M257" s="8">
-        <v>1</v>
-      </c>
-      <c r="N257" s="8">
-        <v>1</v>
-      </c>
-      <c r="O257" s="8"/>
-      <c r="P257" s="8">
-        <v>1</v>
-      </c>
-      <c r="Q257" s="8">
-        <v>1</v>
-      </c>
-      <c r="R257" s="8">
-        <v>1</v>
-      </c>
-      <c r="S257" s="8"/>
-      <c r="T257" s="8">
-        <v>1</v>
-      </c>
-      <c r="U257" s="8"/>
-      <c r="V257" s="8"/>
-      <c r="W257" s="8"/>
-      <c r="X257" s="8"/>
-      <c r="Y257" s="8">
-        <v>1</v>
-      </c>
-      <c r="Z257" s="8"/>
-      <c r="AA257" s="8"/>
-      <c r="AB257" s="8"/>
+      <c r="C257" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D257" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G257">
+        <v>1</v>
+      </c>
+      <c r="H257">
+        <v>1</v>
+      </c>
+      <c r="I257">
+        <v>1</v>
+      </c>
+      <c r="M257">
+        <v>1</v>
+      </c>
+      <c r="N257">
+        <v>1</v>
+      </c>
+      <c r="P257">
+        <v>1</v>
+      </c>
+      <c r="Q257">
+        <v>1</v>
+      </c>
+      <c r="R257">
+        <v>1</v>
+      </c>
+      <c r="T257">
+        <v>1</v>
+      </c>
+      <c r="Y257">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AB257" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:AC257" xr:uid="{E935C717-A0A0-4754-9512-CFF356DAFA88}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Control Unit testing complete
</commit_message>
<xml_diff>
--- a/opcode to control bits.xlsx
+++ b/opcode to control bits.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vjrai\Documents\SC8bCPU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2710C16F-B066-4BEB-9302-DC0F8E9FC3AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D78E6B4-B07F-4959-B5C8-19840A7D8B72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="13875" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -14165,10 +14165,10 @@
   <dimension ref="A1:AC257"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="F85" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E173" sqref="E173"/>
+      <selection pane="bottomRight" activeCell="O98" sqref="O98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -17124,6 +17124,9 @@
       <c r="G94">
         <v>1</v>
       </c>
+      <c r="O94">
+        <v>1</v>
+      </c>
       <c r="P94">
         <v>1</v>
       </c>
@@ -17159,6 +17162,9 @@
       <c r="N95">
         <v>1</v>
       </c>
+      <c r="O95">
+        <v>1</v>
+      </c>
       <c r="P95">
         <v>1</v>
       </c>
@@ -17194,6 +17200,9 @@
       <c r="M96">
         <v>1</v>
       </c>
+      <c r="O96">
+        <v>1</v>
+      </c>
       <c r="P96">
         <v>1</v>
       </c>
@@ -17235,6 +17244,9 @@
       <c r="N97">
         <v>1</v>
       </c>
+      <c r="O97">
+        <v>1</v>
+      </c>
       <c r="P97">
         <v>1</v>
       </c>
@@ -22103,6 +22115,9 @@
       <c r="G254">
         <v>1</v>
       </c>
+      <c r="O254">
+        <v>1</v>
+      </c>
       <c r="P254">
         <v>1</v>
       </c>
@@ -22141,6 +22156,9 @@
       <c r="N255">
         <v>1</v>
       </c>
+      <c r="O255">
+        <v>1</v>
+      </c>
       <c r="P255">
         <v>1</v>
       </c>
@@ -22179,6 +22197,9 @@
       <c r="M256">
         <v>1</v>
       </c>
+      <c r="O256">
+        <v>1</v>
+      </c>
       <c r="P256">
         <v>1</v>
       </c>
@@ -22221,6 +22242,9 @@
         <v>1</v>
       </c>
       <c r="N257">
+        <v>1</v>
+      </c>
+      <c r="O257">
         <v>1</v>
       </c>
       <c r="P257">

</xml_diff>

<commit_message>
Rename to v4, Update DMEM, remove X_Sel
</commit_message>
<xml_diff>
--- a/opcode to control bits.xlsx
+++ b/opcode to control bits.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vjrai\Documents\SC8bCPU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A85B632F-CD6C-4713-AE24-DE58A7B701D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69D38736-236C-4681-BA4C-E099A96850C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="13875" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'v1'!$A$1:$X$257</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'v2'!$A$1:$AA$257</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'v3'!$A$1:$AC$257</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'v4'!$A$1:$AB$257</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'v4'!$A$1:$AA$257</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4272" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4270" uniqueCount="116">
   <si>
     <t>Instruction</t>
   </si>
@@ -443,13 +443,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -22286,13 +22283,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67B22997-F6D9-4937-9D98-6675577120D6}">
-  <dimension ref="A1:AB257"/>
+  <dimension ref="A1:AA257"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="O119" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H24" sqref="H24"/>
+      <selection pane="bottomRight" activeCell="AB59" sqref="AB59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -22315,10 +22312,9 @@
     <col min="24" max="24" width="11.9296875" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="8.46484375" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="9.9296875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="7.9296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -22398,13 +22394,10 @@
         <v>84</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="AB1" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>30</v>
       </c>
@@ -22427,7 +22420,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>30</v>
       </c>
@@ -22453,7 +22446,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>30</v>
       </c>
@@ -22479,7 +22472,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>30</v>
       </c>
@@ -22508,7 +22501,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>32</v>
       </c>
@@ -22531,7 +22524,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>32</v>
       </c>
@@ -22557,7 +22550,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>32</v>
       </c>
@@ -22583,7 +22576,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>32</v>
       </c>
@@ -22612,7 +22605,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>34</v>
       </c>
@@ -22631,15 +22624,6 @@
       <c r="G10">
         <v>1</v>
       </c>
-      <c r="M10">
-        <v>1</v>
-      </c>
-      <c r="N10">
-        <v>1</v>
-      </c>
-      <c r="T10">
-        <v>1</v>
-      </c>
       <c r="W10">
         <v>1</v>
       </c>
@@ -22647,7 +22631,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>34</v>
       </c>
@@ -22669,15 +22653,6 @@
       <c r="I11">
         <v>1</v>
       </c>
-      <c r="M11">
-        <v>1</v>
-      </c>
-      <c r="N11">
-        <v>1</v>
-      </c>
-      <c r="T11">
-        <v>1</v>
-      </c>
       <c r="W11">
         <v>1</v>
       </c>
@@ -22685,7 +22660,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>34</v>
       </c>
@@ -22707,15 +22682,6 @@
       <c r="H12">
         <v>1</v>
       </c>
-      <c r="M12">
-        <v>1</v>
-      </c>
-      <c r="N12">
-        <v>1</v>
-      </c>
-      <c r="T12">
-        <v>1</v>
-      </c>
       <c r="W12">
         <v>1</v>
       </c>
@@ -22723,7 +22689,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
         <v>34</v>
       </c>
@@ -22748,15 +22714,6 @@
       <c r="I13">
         <v>1</v>
       </c>
-      <c r="M13">
-        <v>1</v>
-      </c>
-      <c r="N13">
-        <v>1</v>
-      </c>
-      <c r="T13">
-        <v>1</v>
-      </c>
       <c r="W13">
         <v>1</v>
       </c>
@@ -22764,7 +22721,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
         <v>24</v>
       </c>
@@ -22781,7 +22738,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
         <v>24</v>
       </c>
@@ -22798,7 +22755,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>24</v>
       </c>
@@ -22993,15 +22950,6 @@
       <c r="D26" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="M26">
-        <v>1</v>
-      </c>
-      <c r="N26">
-        <v>1</v>
-      </c>
-      <c r="T26">
-        <v>1</v>
-      </c>
       <c r="V26">
         <v>1</v>
       </c>
@@ -23028,15 +22976,6 @@
       <c r="L27">
         <v>1</v>
       </c>
-      <c r="M27">
-        <v>1</v>
-      </c>
-      <c r="N27">
-        <v>1</v>
-      </c>
-      <c r="T27">
-        <v>1</v>
-      </c>
       <c r="V27">
         <v>1</v>
       </c>
@@ -23063,15 +23002,6 @@
       <c r="K28">
         <v>1</v>
       </c>
-      <c r="M28">
-        <v>1</v>
-      </c>
-      <c r="N28">
-        <v>1</v>
-      </c>
-      <c r="T28">
-        <v>1</v>
-      </c>
       <c r="V28">
         <v>1</v>
       </c>
@@ -23101,15 +23031,6 @@
       <c r="L29">
         <v>1</v>
       </c>
-      <c r="M29">
-        <v>1</v>
-      </c>
-      <c r="N29">
-        <v>1</v>
-      </c>
-      <c r="T29">
-        <v>1</v>
-      </c>
       <c r="V29">
         <v>1</v>
       </c>
@@ -23204,7 +23125,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A33" s="1" t="s">
         <v>52</v>
       </c>
@@ -23236,7 +23157,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A34" s="1" t="s">
         <v>102</v>
       </c>
@@ -23262,7 +23183,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A35" s="1" t="s">
         <v>102</v>
       </c>
@@ -23294,7 +23215,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A36" s="1" t="s">
         <v>102</v>
       </c>
@@ -23326,7 +23247,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A37" s="1" t="s">
         <v>102</v>
       </c>
@@ -23364,7 +23285,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A38" s="1" t="s">
         <v>101</v>
       </c>
@@ -23393,7 +23314,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A39" s="1" t="s">
         <v>101</v>
       </c>
@@ -23428,7 +23349,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A40" s="1" t="s">
         <v>101</v>
       </c>
@@ -23463,7 +23384,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A41" s="1" t="s">
         <v>101</v>
       </c>
@@ -23504,7 +23425,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A42" s="1" t="s">
         <v>43</v>
       </c>
@@ -23523,14 +23444,14 @@
       <c r="S42">
         <v>1</v>
       </c>
+      <c r="W42">
+        <v>1</v>
+      </c>
       <c r="Y42">
         <v>1</v>
       </c>
-      <c r="AA42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:27" x14ac:dyDescent="0.45">
+    </row>
+    <row r="43" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A43" s="1" t="s">
         <v>43</v>
       </c>
@@ -23555,14 +23476,14 @@
       <c r="S43">
         <v>1</v>
       </c>
+      <c r="W43">
+        <v>1</v>
+      </c>
       <c r="Y43">
         <v>1</v>
       </c>
-      <c r="AA43">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:27" x14ac:dyDescent="0.45">
+    </row>
+    <row r="44" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A44" s="1" t="s">
         <v>43</v>
       </c>
@@ -23587,14 +23508,14 @@
       <c r="S44">
         <v>1</v>
       </c>
+      <c r="W44">
+        <v>1</v>
+      </c>
       <c r="Y44">
         <v>1</v>
       </c>
-      <c r="AA44">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:27" x14ac:dyDescent="0.45">
+    </row>
+    <row r="45" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A45" s="1" t="s">
         <v>43</v>
       </c>
@@ -23625,14 +23546,14 @@
       <c r="S45">
         <v>1</v>
       </c>
+      <c r="W45">
+        <v>1</v>
+      </c>
       <c r="Y45">
         <v>1</v>
       </c>
-      <c r="AA45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:27" x14ac:dyDescent="0.45">
+    </row>
+    <row r="46" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A46" s="1" t="s">
         <v>54</v>
       </c>
@@ -23652,7 +23573,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A47" s="1" t="s">
         <v>54</v>
       </c>
@@ -23675,7 +23596,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A48" s="1" t="s">
         <v>54</v>
       </c>
@@ -23698,7 +23619,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A49" s="1" t="s">
         <v>54</v>
       </c>
@@ -23724,7 +23645,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A50" s="1" t="s">
         <v>103</v>
       </c>
@@ -23753,7 +23674,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A51" s="1" t="s">
         <v>103</v>
       </c>
@@ -23788,7 +23709,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A52" s="1" t="s">
         <v>103</v>
       </c>
@@ -23823,7 +23744,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A53" s="1" t="s">
         <v>103</v>
       </c>
@@ -23864,7 +23785,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A54" s="1" t="s">
         <v>104</v>
       </c>
@@ -23896,7 +23817,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A55" s="1" t="s">
         <v>104</v>
       </c>
@@ -23934,7 +23855,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A56" s="1" t="s">
         <v>104</v>
       </c>
@@ -23972,7 +23893,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A57" s="1" t="s">
         <v>104</v>
       </c>
@@ -24016,7 +23937,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A58" s="1" t="s">
         <v>47</v>
       </c>
@@ -24038,14 +23959,14 @@
       <c r="S58">
         <v>1</v>
       </c>
+      <c r="W58">
+        <v>1</v>
+      </c>
       <c r="Y58">
         <v>1</v>
       </c>
-      <c r="AA58">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:27" x14ac:dyDescent="0.45">
+    </row>
+    <row r="59" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A59" s="1" t="s">
         <v>47</v>
       </c>
@@ -24073,14 +23994,14 @@
       <c r="S59">
         <v>1</v>
       </c>
+      <c r="W59">
+        <v>1</v>
+      </c>
       <c r="Y59">
         <v>1</v>
       </c>
-      <c r="AA59">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:27" x14ac:dyDescent="0.45">
+    </row>
+    <row r="60" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A60" s="1" t="s">
         <v>47</v>
       </c>
@@ -24108,14 +24029,14 @@
       <c r="S60">
         <v>1</v>
       </c>
+      <c r="W60">
+        <v>1</v>
+      </c>
       <c r="Y60">
         <v>1</v>
       </c>
-      <c r="AA60">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:27" x14ac:dyDescent="0.45">
+    </row>
+    <row r="61" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A61" s="1" t="s">
         <v>47</v>
       </c>
@@ -24149,14 +24070,14 @@
       <c r="S61">
         <v>1</v>
       </c>
+      <c r="W61">
+        <v>1</v>
+      </c>
       <c r="Y61">
         <v>1</v>
       </c>
-      <c r="AA61">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:27" x14ac:dyDescent="0.45">
+    </row>
+    <row r="62" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A62" s="1" t="s">
         <v>98</v>
       </c>
@@ -24185,7 +24106,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A63" s="1" t="s">
         <v>98</v>
       </c>
@@ -24220,7 +24141,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A64" s="1" t="s">
         <v>98</v>
       </c>
@@ -25884,7 +25805,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A113" s="1" t="s">
         <v>94</v>
       </c>
@@ -25928,7 +25849,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A114" s="1" t="s">
         <v>97</v>
       </c>
@@ -25944,11 +25865,11 @@
       <c r="Y114">
         <v>1</v>
       </c>
-      <c r="AB114">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="115" spans="1:28" x14ac:dyDescent="0.45">
+      <c r="AA114">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A115" s="1" t="s">
         <v>97</v>
       </c>
@@ -25967,11 +25888,11 @@
       <c r="Y115">
         <v>1</v>
       </c>
-      <c r="AB115">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="116" spans="1:28" x14ac:dyDescent="0.45">
+      <c r="AA115">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A116" s="1" t="s">
         <v>97</v>
       </c>
@@ -25990,11 +25911,11 @@
       <c r="Y116">
         <v>1</v>
       </c>
-      <c r="AB116">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="117" spans="1:28" x14ac:dyDescent="0.45">
+      <c r="AA116">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A117" s="1" t="s">
         <v>97</v>
       </c>
@@ -26016,11 +25937,11 @@
       <c r="Y117">
         <v>1</v>
       </c>
-      <c r="AB117">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="118" spans="1:28" x14ac:dyDescent="0.45">
+      <c r="AA117">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A118" s="1" t="s">
         <v>97</v>
       </c>
@@ -26039,11 +25960,11 @@
       <c r="Y118">
         <v>1</v>
       </c>
-      <c r="AB118">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="119" spans="1:28" x14ac:dyDescent="0.45">
+      <c r="AA118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A119" s="1" t="s">
         <v>97</v>
       </c>
@@ -26065,11 +25986,11 @@
       <c r="Y119">
         <v>1</v>
       </c>
-      <c r="AB119">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="120" spans="1:28" x14ac:dyDescent="0.45">
+      <c r="AA119">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A120" s="1" t="s">
         <v>97</v>
       </c>
@@ -26091,11 +26012,11 @@
       <c r="Y120">
         <v>1</v>
       </c>
-      <c r="AB120">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="121" spans="1:28" x14ac:dyDescent="0.45">
+      <c r="AA120">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A121" s="1" t="s">
         <v>97</v>
       </c>
@@ -26120,11 +26041,11 @@
       <c r="Y121">
         <v>1</v>
       </c>
-      <c r="AB121">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="122" spans="1:28" x14ac:dyDescent="0.45">
+      <c r="AA121">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A122" s="1" t="s">
         <v>97</v>
       </c>
@@ -26143,11 +26064,11 @@
       <c r="Y122">
         <v>1</v>
       </c>
-      <c r="AB122">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="123" spans="1:28" x14ac:dyDescent="0.45">
+      <c r="AA122">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A123" s="1" t="s">
         <v>97</v>
       </c>
@@ -26169,11 +26090,11 @@
       <c r="Y123">
         <v>1</v>
       </c>
-      <c r="AB123">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="124" spans="1:28" x14ac:dyDescent="0.45">
+      <c r="AA123">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A124" s="1" t="s">
         <v>97</v>
       </c>
@@ -26195,11 +26116,11 @@
       <c r="Y124">
         <v>1</v>
       </c>
-      <c r="AB124">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="125" spans="1:28" x14ac:dyDescent="0.45">
+      <c r="AA124">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A125" s="1" t="s">
         <v>97</v>
       </c>
@@ -26224,11 +26145,11 @@
       <c r="Y125">
         <v>1</v>
       </c>
-      <c r="AB125">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="126" spans="1:28" x14ac:dyDescent="0.45">
+      <c r="AA125">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A126" s="1" t="s">
         <v>97</v>
       </c>
@@ -26250,11 +26171,11 @@
       <c r="Y126">
         <v>1</v>
       </c>
-      <c r="AB126">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="127" spans="1:28" x14ac:dyDescent="0.45">
+      <c r="AA126">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A127" s="1" t="s">
         <v>97</v>
       </c>
@@ -26279,11 +26200,11 @@
       <c r="Y127">
         <v>1</v>
       </c>
-      <c r="AB127">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="128" spans="1:28" x14ac:dyDescent="0.45">
+      <c r="AA127">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A128" s="1" t="s">
         <v>97</v>
       </c>
@@ -26308,11 +26229,11 @@
       <c r="Y128">
         <v>1</v>
       </c>
-      <c r="AB128">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="129" spans="1:28" x14ac:dyDescent="0.45">
+      <c r="AA128">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A129" s="1" t="s">
         <v>97</v>
       </c>
@@ -26340,11 +26261,11 @@
       <c r="Y129">
         <v>1</v>
       </c>
-      <c r="AB129">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="130" spans="1:28" x14ac:dyDescent="0.45">
+      <c r="AA129">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A130" s="1" t="s">
         <v>56</v>
       </c>
@@ -26370,7 +26291,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A131" s="1" t="s">
         <v>56</v>
       </c>
@@ -26399,7 +26320,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A132" s="1" t="s">
         <v>56</v>
       </c>
@@ -26428,7 +26349,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A133" s="1" t="s">
         <v>56</v>
       </c>
@@ -26460,7 +26381,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A134" s="1" t="s">
         <v>58</v>
       </c>
@@ -26489,7 +26410,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A135" s="1" t="s">
         <v>58</v>
       </c>
@@ -26521,7 +26442,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A136" s="1" t="s">
         <v>58</v>
       </c>
@@ -26553,7 +26474,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A137" s="1" t="s">
         <v>58</v>
       </c>
@@ -26588,7 +26509,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A138" s="1" t="s">
         <v>60</v>
       </c>
@@ -26607,14 +26528,14 @@
       <c r="S138">
         <v>1</v>
       </c>
+      <c r="W138">
+        <v>1</v>
+      </c>
       <c r="Y138">
         <v>1</v>
       </c>
-      <c r="AA138">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="139" spans="1:28" x14ac:dyDescent="0.45">
+    </row>
+    <row r="139" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A139" s="1" t="s">
         <v>60</v>
       </c>
@@ -26636,14 +26557,14 @@
       <c r="S139">
         <v>1</v>
       </c>
+      <c r="W139">
+        <v>1</v>
+      </c>
       <c r="Y139">
         <v>1</v>
       </c>
-      <c r="AA139">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="140" spans="1:28" x14ac:dyDescent="0.45">
+    </row>
+    <row r="140" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A140" s="1" t="s">
         <v>60</v>
       </c>
@@ -26665,14 +26586,14 @@
       <c r="S140">
         <v>1</v>
       </c>
+      <c r="W140">
+        <v>1</v>
+      </c>
       <c r="Y140">
         <v>1</v>
       </c>
-      <c r="AA140">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="141" spans="1:28" x14ac:dyDescent="0.45">
+    </row>
+    <row r="141" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A141" s="1" t="s">
         <v>60</v>
       </c>
@@ -26697,14 +26618,14 @@
       <c r="S141">
         <v>1</v>
       </c>
+      <c r="W141">
+        <v>1</v>
+      </c>
       <c r="Y141">
         <v>1</v>
       </c>
-      <c r="AA141">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="142" spans="1:28" x14ac:dyDescent="0.45">
+    </row>
+    <row r="142" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A142" s="1" t="s">
         <v>61</v>
       </c>
@@ -26724,7 +26645,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A143" s="1" t="s">
         <v>61</v>
       </c>
@@ -26744,7 +26665,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="144" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A144" s="1" t="s">
         <v>61</v>
       </c>
@@ -27084,7 +27005,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="161" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A161" s="1" t="s">
         <v>89</v>
       </c>
@@ -27104,7 +27025,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="162" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A162" s="1" t="s">
         <v>105</v>
       </c>
@@ -27130,7 +27051,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="163" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="163" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A163" s="1" t="s">
         <v>105</v>
       </c>
@@ -27162,7 +27083,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="164" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="164" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A164" s="1" t="s">
         <v>105</v>
       </c>
@@ -27194,7 +27115,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="165" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="165" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A165" s="1" t="s">
         <v>105</v>
       </c>
@@ -27232,7 +27153,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="166" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="166" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A166" s="1" t="s">
         <v>106</v>
       </c>
@@ -27261,7 +27182,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="167" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="167" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A167" s="1" t="s">
         <v>106</v>
       </c>
@@ -27296,7 +27217,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="168" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="168" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A168" s="1" t="s">
         <v>106</v>
       </c>
@@ -27331,7 +27252,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="169" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="169" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A169" s="1" t="s">
         <v>106</v>
       </c>
@@ -27372,7 +27293,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="170" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="170" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A170" s="1" t="s">
         <v>71</v>
       </c>
@@ -27391,14 +27312,14 @@
       <c r="R170">
         <v>1</v>
       </c>
+      <c r="W170">
+        <v>1</v>
+      </c>
       <c r="Y170">
         <v>1</v>
       </c>
-      <c r="AA170">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="171" spans="1:27" x14ac:dyDescent="0.45">
+    </row>
+    <row r="171" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A171" s="1" t="s">
         <v>71</v>
       </c>
@@ -27423,14 +27344,14 @@
       <c r="R171">
         <v>1</v>
       </c>
+      <c r="W171">
+        <v>1</v>
+      </c>
       <c r="Y171">
         <v>1</v>
       </c>
-      <c r="AA171">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="172" spans="1:27" x14ac:dyDescent="0.45">
+    </row>
+    <row r="172" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A172" s="1" t="s">
         <v>71</v>
       </c>
@@ -27455,14 +27376,14 @@
       <c r="R172">
         <v>1</v>
       </c>
+      <c r="W172">
+        <v>1</v>
+      </c>
       <c r="Y172">
         <v>1</v>
       </c>
-      <c r="AA172">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="173" spans="1:27" x14ac:dyDescent="0.45">
+    </row>
+    <row r="173" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A173" s="1" t="s">
         <v>71</v>
       </c>
@@ -27493,14 +27414,14 @@
       <c r="R173">
         <v>1</v>
       </c>
+      <c r="W173">
+        <v>1</v>
+      </c>
       <c r="Y173">
         <v>1</v>
       </c>
-      <c r="AA173">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="174" spans="1:27" x14ac:dyDescent="0.45">
+    </row>
+    <row r="174" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A174" s="1" t="s">
         <v>111</v>
       </c>
@@ -27523,7 +27444,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="175" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="175" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A175" s="1" t="s">
         <v>111</v>
       </c>
@@ -27552,7 +27473,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="176" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="176" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A176" s="1" t="s">
         <v>111</v>
       </c>
@@ -27616,519 +27537,519 @@
         <v>1</v>
       </c>
     </row>
-    <row r="178" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A178" s="3" t="s">
+    <row r="178" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A178" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B178" s="3" t="s">
+      <c r="B178" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C178" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D178" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G178" s="5">
-        <v>1</v>
-      </c>
-      <c r="R178" s="5">
-        <v>1</v>
-      </c>
-      <c r="Y178" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="179" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A179" s="3" t="s">
+      <c r="C178" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D178" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G178">
+        <v>1</v>
+      </c>
+      <c r="R178">
+        <v>1</v>
+      </c>
+      <c r="Y178">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="179" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A179" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B179" s="3" t="s">
+      <c r="B179" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C179" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D179" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="G179" s="5">
-        <v>1</v>
-      </c>
-      <c r="I179" s="5">
-        <v>1</v>
-      </c>
-      <c r="N179" s="5">
-        <v>1</v>
-      </c>
-      <c r="R179" s="5">
-        <v>1</v>
-      </c>
-      <c r="Y179" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="180" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A180" s="3" t="s">
+      <c r="C179" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D179" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G179">
+        <v>1</v>
+      </c>
+      <c r="I179">
+        <v>1</v>
+      </c>
+      <c r="N179">
+        <v>1</v>
+      </c>
+      <c r="R179">
+        <v>1</v>
+      </c>
+      <c r="Y179">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="180" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A180" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B180" s="3" t="s">
+      <c r="B180" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C180" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D180" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G180" s="5">
-        <v>1</v>
-      </c>
-      <c r="H180" s="5">
-        <v>1</v>
-      </c>
-      <c r="M180" s="5">
-        <v>1</v>
-      </c>
-      <c r="R180" s="5">
-        <v>1</v>
-      </c>
-      <c r="Y180" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="181" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A181" s="3" t="s">
+      <c r="C180" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D180" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G180">
+        <v>1</v>
+      </c>
+      <c r="H180">
+        <v>1</v>
+      </c>
+      <c r="M180">
+        <v>1</v>
+      </c>
+      <c r="R180">
+        <v>1</v>
+      </c>
+      <c r="Y180">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="181" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A181" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B181" s="3" t="s">
+      <c r="B181" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C181" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D181" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="G181" s="5">
-        <v>1</v>
-      </c>
-      <c r="H181" s="5">
-        <v>1</v>
-      </c>
-      <c r="I181" s="5">
-        <v>1</v>
-      </c>
-      <c r="M181" s="5">
-        <v>1</v>
-      </c>
-      <c r="N181" s="5">
-        <v>1</v>
-      </c>
-      <c r="R181" s="5">
-        <v>1</v>
-      </c>
-      <c r="Y181" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="182" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A182" s="3" t="s">
+      <c r="C181" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D181" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G181">
+        <v>1</v>
+      </c>
+      <c r="H181">
+        <v>1</v>
+      </c>
+      <c r="I181">
+        <v>1</v>
+      </c>
+      <c r="M181">
+        <v>1</v>
+      </c>
+      <c r="N181">
+        <v>1</v>
+      </c>
+      <c r="R181">
+        <v>1</v>
+      </c>
+      <c r="Y181">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="182" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A182" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B182" s="3" t="s">
+      <c r="B182" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C182" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D182" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G182" s="5">
-        <v>1</v>
-      </c>
-      <c r="L182" s="5">
-        <v>1</v>
-      </c>
-      <c r="R182" s="5">
-        <v>1</v>
-      </c>
-      <c r="Y182" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="183" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A183" s="3" t="s">
+      <c r="C182" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D182" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G182">
+        <v>1</v>
+      </c>
+      <c r="L182">
+        <v>1</v>
+      </c>
+      <c r="R182">
+        <v>1</v>
+      </c>
+      <c r="Y182">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="183" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A183" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B183" s="3" t="s">
+      <c r="B183" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C183" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D183" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="G183" s="5">
-        <v>1</v>
-      </c>
-      <c r="I183" s="5">
-        <v>1</v>
-      </c>
-      <c r="L183" s="5">
-        <v>1</v>
-      </c>
-      <c r="N183" s="5">
-        <v>1</v>
-      </c>
-      <c r="R183" s="5">
-        <v>1</v>
-      </c>
-      <c r="Y183" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="184" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A184" s="3" t="s">
+      <c r="C183" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D183" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G183">
+        <v>1</v>
+      </c>
+      <c r="I183">
+        <v>1</v>
+      </c>
+      <c r="L183">
+        <v>1</v>
+      </c>
+      <c r="N183">
+        <v>1</v>
+      </c>
+      <c r="R183">
+        <v>1</v>
+      </c>
+      <c r="Y183">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="184" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A184" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B184" s="3" t="s">
+      <c r="B184" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C184" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D184" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G184" s="5">
-        <v>1</v>
-      </c>
-      <c r="H184" s="5">
-        <v>1</v>
-      </c>
-      <c r="L184" s="5">
-        <v>1</v>
-      </c>
-      <c r="M184" s="5">
-        <v>1</v>
-      </c>
-      <c r="R184" s="5">
-        <v>1</v>
-      </c>
-      <c r="Y184" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="185" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A185" s="3" t="s">
+      <c r="C184" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D184" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G184">
+        <v>1</v>
+      </c>
+      <c r="H184">
+        <v>1</v>
+      </c>
+      <c r="L184">
+        <v>1</v>
+      </c>
+      <c r="M184">
+        <v>1</v>
+      </c>
+      <c r="R184">
+        <v>1</v>
+      </c>
+      <c r="Y184">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="185" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A185" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B185" s="3" t="s">
+      <c r="B185" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C185" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D185" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="G185" s="5">
-        <v>1</v>
-      </c>
-      <c r="H185" s="5">
-        <v>1</v>
-      </c>
-      <c r="I185" s="5">
-        <v>1</v>
-      </c>
-      <c r="L185" s="5">
-        <v>1</v>
-      </c>
-      <c r="M185" s="5">
-        <v>1</v>
-      </c>
-      <c r="N185" s="5">
-        <v>1</v>
-      </c>
-      <c r="R185" s="5">
-        <v>1</v>
-      </c>
-      <c r="Y185" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="186" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A186" s="3" t="s">
+      <c r="C185" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D185" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G185">
+        <v>1</v>
+      </c>
+      <c r="H185">
+        <v>1</v>
+      </c>
+      <c r="I185">
+        <v>1</v>
+      </c>
+      <c r="L185">
+        <v>1</v>
+      </c>
+      <c r="M185">
+        <v>1</v>
+      </c>
+      <c r="N185">
+        <v>1</v>
+      </c>
+      <c r="R185">
+        <v>1</v>
+      </c>
+      <c r="Y185">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="186" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A186" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B186" s="3" t="s">
+      <c r="B186" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C186" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D186" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G186" s="5">
-        <v>1</v>
-      </c>
-      <c r="K186" s="5">
-        <v>1</v>
-      </c>
-      <c r="R186" s="5">
-        <v>1</v>
-      </c>
-      <c r="Y186" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="187" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A187" s="3" t="s">
+      <c r="C186" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D186" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G186">
+        <v>1</v>
+      </c>
+      <c r="K186">
+        <v>1</v>
+      </c>
+      <c r="R186">
+        <v>1</v>
+      </c>
+      <c r="Y186">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="187" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A187" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B187" s="3" t="s">
+      <c r="B187" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C187" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D187" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="G187" s="5">
-        <v>1</v>
-      </c>
-      <c r="I187" s="5">
-        <v>1</v>
-      </c>
-      <c r="K187" s="5">
-        <v>1</v>
-      </c>
-      <c r="N187" s="5">
-        <v>1</v>
-      </c>
-      <c r="R187" s="5">
-        <v>1</v>
-      </c>
-      <c r="Y187" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="188" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A188" s="3" t="s">
+      <c r="C187" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D187" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G187">
+        <v>1</v>
+      </c>
+      <c r="I187">
+        <v>1</v>
+      </c>
+      <c r="K187">
+        <v>1</v>
+      </c>
+      <c r="N187">
+        <v>1</v>
+      </c>
+      <c r="R187">
+        <v>1</v>
+      </c>
+      <c r="Y187">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="188" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A188" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B188" s="3" t="s">
+      <c r="B188" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C188" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D188" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G188" s="5">
-        <v>1</v>
-      </c>
-      <c r="H188" s="5">
-        <v>1</v>
-      </c>
-      <c r="K188" s="5">
-        <v>1</v>
-      </c>
-      <c r="M188" s="5">
-        <v>1</v>
-      </c>
-      <c r="R188" s="5">
-        <v>1</v>
-      </c>
-      <c r="Y188" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="189" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A189" s="3" t="s">
+      <c r="C188" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D188" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G188">
+        <v>1</v>
+      </c>
+      <c r="H188">
+        <v>1</v>
+      </c>
+      <c r="K188">
+        <v>1</v>
+      </c>
+      <c r="M188">
+        <v>1</v>
+      </c>
+      <c r="R188">
+        <v>1</v>
+      </c>
+      <c r="Y188">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="189" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A189" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B189" s="3" t="s">
+      <c r="B189" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C189" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D189" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="G189" s="5">
-        <v>1</v>
-      </c>
-      <c r="H189" s="5">
-        <v>1</v>
-      </c>
-      <c r="I189" s="5">
-        <v>1</v>
-      </c>
-      <c r="K189" s="5">
-        <v>1</v>
-      </c>
-      <c r="M189" s="5">
-        <v>1</v>
-      </c>
-      <c r="N189" s="5">
-        <v>1</v>
-      </c>
-      <c r="R189" s="5">
-        <v>1</v>
-      </c>
-      <c r="Y189" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="190" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A190" s="3" t="s">
+      <c r="C189" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D189" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G189">
+        <v>1</v>
+      </c>
+      <c r="H189">
+        <v>1</v>
+      </c>
+      <c r="I189">
+        <v>1</v>
+      </c>
+      <c r="K189">
+        <v>1</v>
+      </c>
+      <c r="M189">
+        <v>1</v>
+      </c>
+      <c r="N189">
+        <v>1</v>
+      </c>
+      <c r="R189">
+        <v>1</v>
+      </c>
+      <c r="Y189">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="190" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A190" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B190" s="3" t="s">
+      <c r="B190" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C190" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D190" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G190" s="5">
-        <v>1</v>
-      </c>
-      <c r="K190" s="5">
-        <v>1</v>
-      </c>
-      <c r="L190" s="5">
-        <v>1</v>
-      </c>
-      <c r="R190" s="5">
-        <v>1</v>
-      </c>
-      <c r="Y190" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="191" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A191" s="3" t="s">
+      <c r="C190" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D190" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G190">
+        <v>1</v>
+      </c>
+      <c r="K190">
+        <v>1</v>
+      </c>
+      <c r="L190">
+        <v>1</v>
+      </c>
+      <c r="R190">
+        <v>1</v>
+      </c>
+      <c r="Y190">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="191" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A191" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B191" s="3" t="s">
+      <c r="B191" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C191" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D191" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="G191" s="5">
-        <v>1</v>
-      </c>
-      <c r="I191" s="5">
-        <v>1</v>
-      </c>
-      <c r="K191" s="5">
-        <v>1</v>
-      </c>
-      <c r="L191" s="5">
-        <v>1</v>
-      </c>
-      <c r="N191" s="5">
-        <v>1</v>
-      </c>
-      <c r="R191" s="5">
-        <v>1</v>
-      </c>
-      <c r="Y191" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="192" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A192" s="3" t="s">
+      <c r="C191" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D191" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G191">
+        <v>1</v>
+      </c>
+      <c r="I191">
+        <v>1</v>
+      </c>
+      <c r="K191">
+        <v>1</v>
+      </c>
+      <c r="L191">
+        <v>1</v>
+      </c>
+      <c r="N191">
+        <v>1</v>
+      </c>
+      <c r="R191">
+        <v>1</v>
+      </c>
+      <c r="Y191">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="192" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A192" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B192" s="3" t="s">
+      <c r="B192" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C192" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D192" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G192" s="5">
-        <v>1</v>
-      </c>
-      <c r="H192" s="5">
-        <v>1</v>
-      </c>
-      <c r="K192" s="5">
-        <v>1</v>
-      </c>
-      <c r="L192" s="5">
-        <v>1</v>
-      </c>
-      <c r="M192" s="5">
-        <v>1</v>
-      </c>
-      <c r="R192" s="5">
-        <v>1</v>
-      </c>
-      <c r="Y192" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="193" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A193" s="3" t="s">
+      <c r="C192" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D192" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G192">
+        <v>1</v>
+      </c>
+      <c r="H192">
+        <v>1</v>
+      </c>
+      <c r="K192">
+        <v>1</v>
+      </c>
+      <c r="L192">
+        <v>1</v>
+      </c>
+      <c r="M192">
+        <v>1</v>
+      </c>
+      <c r="R192">
+        <v>1</v>
+      </c>
+      <c r="Y192">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="193" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A193" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B193" s="3" t="s">
+      <c r="B193" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C193" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D193" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="G193" s="5">
-        <v>1</v>
-      </c>
-      <c r="H193" s="5">
-        <v>1</v>
-      </c>
-      <c r="I193" s="5">
-        <v>1</v>
-      </c>
-      <c r="K193" s="5">
-        <v>1</v>
-      </c>
-      <c r="L193" s="5">
-        <v>1</v>
-      </c>
-      <c r="M193" s="5">
-        <v>1</v>
-      </c>
-      <c r="N193" s="5">
-        <v>1</v>
-      </c>
-      <c r="R193" s="5">
-        <v>1</v>
-      </c>
-      <c r="Y193" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="194" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="C193" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D193" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G193">
+        <v>1</v>
+      </c>
+      <c r="H193">
+        <v>1</v>
+      </c>
+      <c r="I193">
+        <v>1</v>
+      </c>
+      <c r="K193">
+        <v>1</v>
+      </c>
+      <c r="L193">
+        <v>1</v>
+      </c>
+      <c r="M193">
+        <v>1</v>
+      </c>
+      <c r="N193">
+        <v>1</v>
+      </c>
+      <c r="R193">
+        <v>1</v>
+      </c>
+      <c r="Y193">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="194" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A194" s="1" t="s">
         <v>107</v>
       </c>
@@ -28154,7 +28075,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="195" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="195" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A195" s="1" t="s">
         <v>107</v>
       </c>
@@ -28186,7 +28107,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="196" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="196" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A196" s="1" t="s">
         <v>107</v>
       </c>
@@ -28218,7 +28139,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="197" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="197" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A197" s="1" t="s">
         <v>107</v>
       </c>
@@ -28256,7 +28177,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="198" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="198" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A198" s="1" t="s">
         <v>108</v>
       </c>
@@ -28285,7 +28206,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="199" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="199" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A199" s="1" t="s">
         <v>108</v>
       </c>
@@ -28320,7 +28241,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="200" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="200" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A200" s="1" t="s">
         <v>108</v>
       </c>
@@ -28355,7 +28276,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="201" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="201" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A201" s="1" t="s">
         <v>108</v>
       </c>
@@ -28396,7 +28317,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="202" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="202" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A202" s="1" t="s">
         <v>75</v>
       </c>
@@ -28415,17 +28336,14 @@
       <c r="Q202">
         <v>1</v>
       </c>
-      <c r="W202" t="s">
-        <v>76</v>
+      <c r="W202">
+        <v>1</v>
       </c>
       <c r="Y202">
         <v>1</v>
       </c>
-      <c r="AA202">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="203" spans="1:27" x14ac:dyDescent="0.45">
+    </row>
+    <row r="203" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A203" s="1" t="s">
         <v>75</v>
       </c>
@@ -28450,14 +28368,14 @@
       <c r="Q203">
         <v>1</v>
       </c>
+      <c r="W203">
+        <v>1</v>
+      </c>
       <c r="Y203">
         <v>1</v>
       </c>
-      <c r="AA203">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="204" spans="1:27" x14ac:dyDescent="0.45">
+    </row>
+    <row r="204" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A204" s="1" t="s">
         <v>75</v>
       </c>
@@ -28482,14 +28400,14 @@
       <c r="Q204">
         <v>1</v>
       </c>
+      <c r="W204">
+        <v>1</v>
+      </c>
       <c r="Y204">
         <v>1</v>
       </c>
-      <c r="AA204">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="205" spans="1:27" x14ac:dyDescent="0.45">
+    </row>
+    <row r="205" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A205" s="1" t="s">
         <v>75</v>
       </c>
@@ -28520,14 +28438,14 @@
       <c r="Q205">
         <v>1</v>
       </c>
+      <c r="W205">
+        <v>1</v>
+      </c>
       <c r="Y205">
         <v>1</v>
       </c>
-      <c r="AA205">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="206" spans="1:27" x14ac:dyDescent="0.45">
+    </row>
+    <row r="206" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A206" s="1" t="s">
         <v>99</v>
       </c>
@@ -28559,7 +28477,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="207" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="207" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A207" s="1" t="s">
         <v>99</v>
       </c>
@@ -28597,7 +28515,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="208" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="208" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A208" s="1" t="s">
         <v>99</v>
       </c>
@@ -28679,519 +28597,519 @@
         <v>1</v>
       </c>
     </row>
-    <row r="210" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A210" s="3" t="s">
+    <row r="210" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A210" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B210" s="3" t="s">
+      <c r="B210" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C210" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D210" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G210" s="5">
-        <v>1</v>
-      </c>
-      <c r="Q210" s="5">
-        <v>1</v>
-      </c>
-      <c r="Y210" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="211" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A211" s="3" t="s">
+      <c r="C210" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D210" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G210">
+        <v>1</v>
+      </c>
+      <c r="Q210">
+        <v>1</v>
+      </c>
+      <c r="Y210">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="211" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A211" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B211" s="3" t="s">
+      <c r="B211" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C211" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D211" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="G211" s="5">
-        <v>1</v>
-      </c>
-      <c r="I211" s="5">
-        <v>1</v>
-      </c>
-      <c r="N211" s="5">
-        <v>1</v>
-      </c>
-      <c r="Q211" s="5">
-        <v>1</v>
-      </c>
-      <c r="Y211" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="212" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A212" s="3" t="s">
+      <c r="C211" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D211" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G211">
+        <v>1</v>
+      </c>
+      <c r="I211">
+        <v>1</v>
+      </c>
+      <c r="N211">
+        <v>1</v>
+      </c>
+      <c r="Q211">
+        <v>1</v>
+      </c>
+      <c r="Y211">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="212" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A212" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B212" s="3" t="s">
+      <c r="B212" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C212" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D212" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G212" s="5">
-        <v>1</v>
-      </c>
-      <c r="H212" s="5">
-        <v>1</v>
-      </c>
-      <c r="M212" s="5">
-        <v>1</v>
-      </c>
-      <c r="Q212" s="5">
-        <v>1</v>
-      </c>
-      <c r="Y212" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="213" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A213" s="3" t="s">
+      <c r="C212" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D212" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G212">
+        <v>1</v>
+      </c>
+      <c r="H212">
+        <v>1</v>
+      </c>
+      <c r="M212">
+        <v>1</v>
+      </c>
+      <c r="Q212">
+        <v>1</v>
+      </c>
+      <c r="Y212">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="213" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A213" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B213" s="3" t="s">
+      <c r="B213" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C213" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D213" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="G213" s="5">
-        <v>1</v>
-      </c>
-      <c r="H213" s="5">
-        <v>1</v>
-      </c>
-      <c r="I213" s="5">
-        <v>1</v>
-      </c>
-      <c r="M213" s="5">
-        <v>1</v>
-      </c>
-      <c r="N213" s="5">
-        <v>1</v>
-      </c>
-      <c r="Q213" s="5">
-        <v>1</v>
-      </c>
-      <c r="Y213" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="214" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A214" s="3" t="s">
+      <c r="C213" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D213" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G213">
+        <v>1</v>
+      </c>
+      <c r="H213">
+        <v>1</v>
+      </c>
+      <c r="I213">
+        <v>1</v>
+      </c>
+      <c r="M213">
+        <v>1</v>
+      </c>
+      <c r="N213">
+        <v>1</v>
+      </c>
+      <c r="Q213">
+        <v>1</v>
+      </c>
+      <c r="Y213">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="214" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A214" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B214" s="3" t="s">
+      <c r="B214" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C214" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D214" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G214" s="5">
-        <v>1</v>
-      </c>
-      <c r="L214" s="5">
-        <v>1</v>
-      </c>
-      <c r="Q214" s="5">
-        <v>1</v>
-      </c>
-      <c r="Y214" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="215" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A215" s="3" t="s">
+      <c r="C214" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D214" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G214">
+        <v>1</v>
+      </c>
+      <c r="L214">
+        <v>1</v>
+      </c>
+      <c r="Q214">
+        <v>1</v>
+      </c>
+      <c r="Y214">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="215" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A215" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B215" s="3" t="s">
+      <c r="B215" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C215" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D215" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="G215" s="5">
-        <v>1</v>
-      </c>
-      <c r="I215" s="5">
-        <v>1</v>
-      </c>
-      <c r="L215" s="5">
-        <v>1</v>
-      </c>
-      <c r="N215" s="5">
-        <v>1</v>
-      </c>
-      <c r="Q215" s="5">
-        <v>1</v>
-      </c>
-      <c r="Y215" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="216" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A216" s="3" t="s">
+      <c r="C215" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D215" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G215">
+        <v>1</v>
+      </c>
+      <c r="I215">
+        <v>1</v>
+      </c>
+      <c r="L215">
+        <v>1</v>
+      </c>
+      <c r="N215">
+        <v>1</v>
+      </c>
+      <c r="Q215">
+        <v>1</v>
+      </c>
+      <c r="Y215">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="216" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A216" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B216" s="3" t="s">
+      <c r="B216" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C216" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D216" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G216" s="5">
-        <v>1</v>
-      </c>
-      <c r="H216" s="5">
-        <v>1</v>
-      </c>
-      <c r="L216" s="5">
-        <v>1</v>
-      </c>
-      <c r="M216" s="5">
-        <v>1</v>
-      </c>
-      <c r="Q216" s="5">
-        <v>1</v>
-      </c>
-      <c r="Y216" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="217" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A217" s="3" t="s">
+      <c r="C216" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D216" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G216">
+        <v>1</v>
+      </c>
+      <c r="H216">
+        <v>1</v>
+      </c>
+      <c r="L216">
+        <v>1</v>
+      </c>
+      <c r="M216">
+        <v>1</v>
+      </c>
+      <c r="Q216">
+        <v>1</v>
+      </c>
+      <c r="Y216">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="217" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A217" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B217" s="3" t="s">
+      <c r="B217" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C217" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D217" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="G217" s="5">
-        <v>1</v>
-      </c>
-      <c r="H217" s="5">
-        <v>1</v>
-      </c>
-      <c r="I217" s="5">
-        <v>1</v>
-      </c>
-      <c r="L217" s="5">
-        <v>1</v>
-      </c>
-      <c r="M217" s="5">
-        <v>1</v>
-      </c>
-      <c r="N217" s="5">
-        <v>1</v>
-      </c>
-      <c r="Q217" s="5">
-        <v>1</v>
-      </c>
-      <c r="Y217" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="218" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A218" s="3" t="s">
+      <c r="C217" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D217" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G217">
+        <v>1</v>
+      </c>
+      <c r="H217">
+        <v>1</v>
+      </c>
+      <c r="I217">
+        <v>1</v>
+      </c>
+      <c r="L217">
+        <v>1</v>
+      </c>
+      <c r="M217">
+        <v>1</v>
+      </c>
+      <c r="N217">
+        <v>1</v>
+      </c>
+      <c r="Q217">
+        <v>1</v>
+      </c>
+      <c r="Y217">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="218" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A218" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B218" s="3" t="s">
+      <c r="B218" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C218" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D218" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G218" s="5">
-        <v>1</v>
-      </c>
-      <c r="K218" s="5">
-        <v>1</v>
-      </c>
-      <c r="Q218" s="5">
-        <v>1</v>
-      </c>
-      <c r="Y218" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="219" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A219" s="3" t="s">
+      <c r="C218" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D218" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G218">
+        <v>1</v>
+      </c>
+      <c r="K218">
+        <v>1</v>
+      </c>
+      <c r="Q218">
+        <v>1</v>
+      </c>
+      <c r="Y218">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="219" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A219" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B219" s="3" t="s">
+      <c r="B219" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C219" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D219" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="G219" s="5">
-        <v>1</v>
-      </c>
-      <c r="I219" s="5">
-        <v>1</v>
-      </c>
-      <c r="K219" s="5">
-        <v>1</v>
-      </c>
-      <c r="N219" s="5">
-        <v>1</v>
-      </c>
-      <c r="Q219" s="5">
-        <v>1</v>
-      </c>
-      <c r="Y219" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="220" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A220" s="3" t="s">
+      <c r="C219" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D219" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G219">
+        <v>1</v>
+      </c>
+      <c r="I219">
+        <v>1</v>
+      </c>
+      <c r="K219">
+        <v>1</v>
+      </c>
+      <c r="N219">
+        <v>1</v>
+      </c>
+      <c r="Q219">
+        <v>1</v>
+      </c>
+      <c r="Y219">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="220" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A220" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B220" s="3" t="s">
+      <c r="B220" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C220" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D220" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G220" s="5">
-        <v>1</v>
-      </c>
-      <c r="H220" s="5">
-        <v>1</v>
-      </c>
-      <c r="K220" s="5">
-        <v>1</v>
-      </c>
-      <c r="M220" s="5">
-        <v>1</v>
-      </c>
-      <c r="Q220" s="5">
-        <v>1</v>
-      </c>
-      <c r="Y220" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="221" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A221" s="3" t="s">
+      <c r="C220" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D220" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G220">
+        <v>1</v>
+      </c>
+      <c r="H220">
+        <v>1</v>
+      </c>
+      <c r="K220">
+        <v>1</v>
+      </c>
+      <c r="M220">
+        <v>1</v>
+      </c>
+      <c r="Q220">
+        <v>1</v>
+      </c>
+      <c r="Y220">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="221" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A221" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B221" s="3" t="s">
+      <c r="B221" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C221" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D221" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="G221" s="5">
-        <v>1</v>
-      </c>
-      <c r="H221" s="5">
-        <v>1</v>
-      </c>
-      <c r="I221" s="5">
-        <v>1</v>
-      </c>
-      <c r="K221" s="5">
-        <v>1</v>
-      </c>
-      <c r="M221" s="5">
-        <v>1</v>
-      </c>
-      <c r="N221" s="5">
-        <v>1</v>
-      </c>
-      <c r="Q221" s="5">
-        <v>1</v>
-      </c>
-      <c r="Y221" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="222" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A222" s="3" t="s">
+      <c r="C221" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D221" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G221">
+        <v>1</v>
+      </c>
+      <c r="H221">
+        <v>1</v>
+      </c>
+      <c r="I221">
+        <v>1</v>
+      </c>
+      <c r="K221">
+        <v>1</v>
+      </c>
+      <c r="M221">
+        <v>1</v>
+      </c>
+      <c r="N221">
+        <v>1</v>
+      </c>
+      <c r="Q221">
+        <v>1</v>
+      </c>
+      <c r="Y221">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="222" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A222" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B222" s="3" t="s">
+      <c r="B222" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C222" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D222" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G222" s="5">
-        <v>1</v>
-      </c>
-      <c r="K222" s="5">
-        <v>1</v>
-      </c>
-      <c r="L222" s="5">
-        <v>1</v>
-      </c>
-      <c r="Q222" s="5">
-        <v>1</v>
-      </c>
-      <c r="Y222" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="223" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A223" s="3" t="s">
+      <c r="C222" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D222" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G222">
+        <v>1</v>
+      </c>
+      <c r="K222">
+        <v>1</v>
+      </c>
+      <c r="L222">
+        <v>1</v>
+      </c>
+      <c r="Q222">
+        <v>1</v>
+      </c>
+      <c r="Y222">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="223" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A223" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B223" s="3" t="s">
+      <c r="B223" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C223" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D223" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="G223" s="5">
-        <v>1</v>
-      </c>
-      <c r="I223" s="5">
-        <v>1</v>
-      </c>
-      <c r="K223" s="5">
-        <v>1</v>
-      </c>
-      <c r="L223" s="5">
-        <v>1</v>
-      </c>
-      <c r="N223" s="5">
-        <v>1</v>
-      </c>
-      <c r="Q223" s="5">
-        <v>1</v>
-      </c>
-      <c r="Y223" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="224" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A224" s="3" t="s">
+      <c r="C223" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D223" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G223">
+        <v>1</v>
+      </c>
+      <c r="I223">
+        <v>1</v>
+      </c>
+      <c r="K223">
+        <v>1</v>
+      </c>
+      <c r="L223">
+        <v>1</v>
+      </c>
+      <c r="N223">
+        <v>1</v>
+      </c>
+      <c r="Q223">
+        <v>1</v>
+      </c>
+      <c r="Y223">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="224" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A224" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B224" s="3" t="s">
+      <c r="B224" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C224" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D224" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G224" s="5">
-        <v>1</v>
-      </c>
-      <c r="H224" s="5">
-        <v>1</v>
-      </c>
-      <c r="K224" s="5">
-        <v>1</v>
-      </c>
-      <c r="L224" s="5">
-        <v>1</v>
-      </c>
-      <c r="M224" s="5">
-        <v>1</v>
-      </c>
-      <c r="Q224" s="5">
-        <v>1</v>
-      </c>
-      <c r="Y224" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="225" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A225" s="3" t="s">
+      <c r="C224" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D224" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G224">
+        <v>1</v>
+      </c>
+      <c r="H224">
+        <v>1</v>
+      </c>
+      <c r="K224">
+        <v>1</v>
+      </c>
+      <c r="L224">
+        <v>1</v>
+      </c>
+      <c r="M224">
+        <v>1</v>
+      </c>
+      <c r="Q224">
+        <v>1</v>
+      </c>
+      <c r="Y224">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="225" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A225" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B225" s="3" t="s">
+      <c r="B225" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C225" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D225" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="G225" s="5">
-        <v>1</v>
-      </c>
-      <c r="H225" s="5">
-        <v>1</v>
-      </c>
-      <c r="I225" s="5">
-        <v>1</v>
-      </c>
-      <c r="K225" s="5">
-        <v>1</v>
-      </c>
-      <c r="L225" s="5">
-        <v>1</v>
-      </c>
-      <c r="M225" s="5">
-        <v>1</v>
-      </c>
-      <c r="N225" s="5">
-        <v>1</v>
-      </c>
-      <c r="Q225" s="5">
-        <v>1</v>
-      </c>
-      <c r="Y225" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="226" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="C225" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D225" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G225">
+        <v>1</v>
+      </c>
+      <c r="H225">
+        <v>1</v>
+      </c>
+      <c r="I225">
+        <v>1</v>
+      </c>
+      <c r="K225">
+        <v>1</v>
+      </c>
+      <c r="L225">
+        <v>1</v>
+      </c>
+      <c r="M225">
+        <v>1</v>
+      </c>
+      <c r="N225">
+        <v>1</v>
+      </c>
+      <c r="Q225">
+        <v>1</v>
+      </c>
+      <c r="Y225">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="226" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A226" s="1" t="s">
         <v>109</v>
       </c>
@@ -29220,7 +29138,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="227" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="227" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A227" s="1" t="s">
         <v>109</v>
       </c>
@@ -29255,7 +29173,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="228" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="228" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A228" s="1" t="s">
         <v>109</v>
       </c>
@@ -29290,7 +29208,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="229" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="229" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A229" s="1" t="s">
         <v>109</v>
       </c>
@@ -29331,7 +29249,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="230" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="230" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A230" s="1" t="s">
         <v>110</v>
       </c>
@@ -29363,7 +29281,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="231" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="231" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A231" s="1" t="s">
         <v>110</v>
       </c>
@@ -29401,7 +29319,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="232" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="232" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A232" s="1" t="s">
         <v>110</v>
       </c>
@@ -29439,7 +29357,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="233" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="233" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A233" s="1" t="s">
         <v>110</v>
       </c>
@@ -29483,7 +29401,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="234" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="234" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A234" s="1" t="s">
         <v>80</v>
       </c>
@@ -29505,14 +29423,14 @@
       <c r="R234">
         <v>1</v>
       </c>
+      <c r="W234">
+        <v>1</v>
+      </c>
       <c r="Y234">
         <v>1</v>
       </c>
-      <c r="AA234">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="235" spans="1:27" x14ac:dyDescent="0.45">
+    </row>
+    <row r="235" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A235" s="1" t="s">
         <v>80</v>
       </c>
@@ -29540,14 +29458,14 @@
       <c r="R235">
         <v>1</v>
       </c>
+      <c r="W235">
+        <v>1</v>
+      </c>
       <c r="Y235">
         <v>1</v>
       </c>
-      <c r="AA235">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="236" spans="1:27" x14ac:dyDescent="0.45">
+    </row>
+    <row r="236" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A236" s="1" t="s">
         <v>80</v>
       </c>
@@ -29575,14 +29493,14 @@
       <c r="R236">
         <v>1</v>
       </c>
+      <c r="W236">
+        <v>1</v>
+      </c>
       <c r="Y236">
         <v>1</v>
       </c>
-      <c r="AA236">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="237" spans="1:27" x14ac:dyDescent="0.45">
+    </row>
+    <row r="237" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A237" s="1" t="s">
         <v>80</v>
       </c>
@@ -29616,14 +29534,14 @@
       <c r="R237">
         <v>1</v>
       </c>
+      <c r="W237">
+        <v>1</v>
+      </c>
       <c r="Y237">
         <v>1</v>
       </c>
-      <c r="AA237">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="238" spans="1:27" x14ac:dyDescent="0.45">
+    </row>
+    <row r="238" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A238" s="1" t="s">
         <v>100</v>
       </c>
@@ -29658,7 +29576,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="239" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="239" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A239" s="1" t="s">
         <v>100</v>
       </c>
@@ -29699,7 +29617,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="240" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="240" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A240" s="1" t="s">
         <v>100</v>
       </c>
@@ -29787,568 +29705,568 @@
         <v>1</v>
       </c>
     </row>
-    <row r="242" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A242" s="3" t="s">
+    <row r="242" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A242" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B242" s="3" t="s">
+      <c r="B242" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C242" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D242" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G242" s="5">
-        <v>1</v>
-      </c>
-      <c r="Q242" s="5">
-        <v>1</v>
-      </c>
-      <c r="R242" s="5">
-        <v>1</v>
-      </c>
-      <c r="Y242" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="243" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A243" s="3" t="s">
+      <c r="C242" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D242" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G242">
+        <v>1</v>
+      </c>
+      <c r="Q242">
+        <v>1</v>
+      </c>
+      <c r="R242">
+        <v>1</v>
+      </c>
+      <c r="Y242">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="243" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A243" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B243" s="3" t="s">
+      <c r="B243" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C243" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D243" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="G243" s="5">
-        <v>1</v>
-      </c>
-      <c r="I243" s="5">
-        <v>1</v>
-      </c>
-      <c r="N243" s="5">
-        <v>1</v>
-      </c>
-      <c r="Q243" s="5">
-        <v>1</v>
-      </c>
-      <c r="R243" s="5">
-        <v>1</v>
-      </c>
-      <c r="Y243" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="244" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A244" s="3" t="s">
+      <c r="C243" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D243" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G243">
+        <v>1</v>
+      </c>
+      <c r="I243">
+        <v>1</v>
+      </c>
+      <c r="N243">
+        <v>1</v>
+      </c>
+      <c r="Q243">
+        <v>1</v>
+      </c>
+      <c r="R243">
+        <v>1</v>
+      </c>
+      <c r="Y243">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="244" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A244" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B244" s="3" t="s">
+      <c r="B244" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C244" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D244" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G244" s="5">
-        <v>1</v>
-      </c>
-      <c r="H244" s="5">
-        <v>1</v>
-      </c>
-      <c r="M244" s="5">
-        <v>1</v>
-      </c>
-      <c r="Q244" s="5">
-        <v>1</v>
-      </c>
-      <c r="R244" s="5">
-        <v>1</v>
-      </c>
-      <c r="Y244" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="245" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A245" s="3" t="s">
+      <c r="C244" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D244" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G244">
+        <v>1</v>
+      </c>
+      <c r="H244">
+        <v>1</v>
+      </c>
+      <c r="M244">
+        <v>1</v>
+      </c>
+      <c r="Q244">
+        <v>1</v>
+      </c>
+      <c r="R244">
+        <v>1</v>
+      </c>
+      <c r="Y244">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="245" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A245" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B245" s="3" t="s">
+      <c r="B245" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C245" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D245" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="G245" s="5">
-        <v>1</v>
-      </c>
-      <c r="H245" s="5">
-        <v>1</v>
-      </c>
-      <c r="I245" s="5">
-        <v>1</v>
-      </c>
-      <c r="M245" s="5">
-        <v>1</v>
-      </c>
-      <c r="N245" s="5">
-        <v>1</v>
-      </c>
-      <c r="Q245" s="5">
-        <v>1</v>
-      </c>
-      <c r="R245" s="5">
-        <v>1</v>
-      </c>
-      <c r="Y245" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="246" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A246" s="3" t="s">
+      <c r="C245" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D245" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G245">
+        <v>1</v>
+      </c>
+      <c r="H245">
+        <v>1</v>
+      </c>
+      <c r="I245">
+        <v>1</v>
+      </c>
+      <c r="M245">
+        <v>1</v>
+      </c>
+      <c r="N245">
+        <v>1</v>
+      </c>
+      <c r="Q245">
+        <v>1</v>
+      </c>
+      <c r="R245">
+        <v>1</v>
+      </c>
+      <c r="Y245">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="246" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A246" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B246" s="3" t="s">
+      <c r="B246" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C246" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D246" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G246" s="5">
-        <v>1</v>
-      </c>
-      <c r="L246" s="5">
-        <v>1</v>
-      </c>
-      <c r="Q246" s="5">
-        <v>1</v>
-      </c>
-      <c r="R246" s="5">
-        <v>1</v>
-      </c>
-      <c r="Y246" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="247" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A247" s="3" t="s">
+      <c r="C246" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D246" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G246">
+        <v>1</v>
+      </c>
+      <c r="L246">
+        <v>1</v>
+      </c>
+      <c r="Q246">
+        <v>1</v>
+      </c>
+      <c r="R246">
+        <v>1</v>
+      </c>
+      <c r="Y246">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="247" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A247" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B247" s="3" t="s">
+      <c r="B247" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C247" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D247" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="G247" s="5">
-        <v>1</v>
-      </c>
-      <c r="I247" s="5">
-        <v>1</v>
-      </c>
-      <c r="L247" s="5">
-        <v>1</v>
-      </c>
-      <c r="N247" s="5">
-        <v>1</v>
-      </c>
-      <c r="Q247" s="5">
-        <v>1</v>
-      </c>
-      <c r="R247" s="5">
-        <v>1</v>
-      </c>
-      <c r="Y247" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="248" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A248" s="3" t="s">
+      <c r="C247" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D247" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G247">
+        <v>1</v>
+      </c>
+      <c r="I247">
+        <v>1</v>
+      </c>
+      <c r="L247">
+        <v>1</v>
+      </c>
+      <c r="N247">
+        <v>1</v>
+      </c>
+      <c r="Q247">
+        <v>1</v>
+      </c>
+      <c r="R247">
+        <v>1</v>
+      </c>
+      <c r="Y247">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="248" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A248" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B248" s="3" t="s">
+      <c r="B248" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C248" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D248" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G248" s="5">
-        <v>1</v>
-      </c>
-      <c r="H248" s="5">
-        <v>1</v>
-      </c>
-      <c r="L248" s="5">
-        <v>1</v>
-      </c>
-      <c r="M248" s="5">
-        <v>1</v>
-      </c>
-      <c r="Q248" s="5">
-        <v>1</v>
-      </c>
-      <c r="R248" s="5">
-        <v>1</v>
-      </c>
-      <c r="Y248" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="249" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A249" s="3" t="s">
+      <c r="C248" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D248" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G248">
+        <v>1</v>
+      </c>
+      <c r="H248">
+        <v>1</v>
+      </c>
+      <c r="L248">
+        <v>1</v>
+      </c>
+      <c r="M248">
+        <v>1</v>
+      </c>
+      <c r="Q248">
+        <v>1</v>
+      </c>
+      <c r="R248">
+        <v>1</v>
+      </c>
+      <c r="Y248">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="249" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A249" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B249" s="3" t="s">
+      <c r="B249" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C249" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D249" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="G249" s="5">
-        <v>1</v>
-      </c>
-      <c r="H249" s="5">
-        <v>1</v>
-      </c>
-      <c r="I249" s="5">
-        <v>1</v>
-      </c>
-      <c r="L249" s="5">
-        <v>1</v>
-      </c>
-      <c r="M249" s="5">
-        <v>1</v>
-      </c>
-      <c r="N249" s="5">
-        <v>1</v>
-      </c>
-      <c r="Q249" s="5">
-        <v>1</v>
-      </c>
-      <c r="R249" s="5">
-        <v>1</v>
-      </c>
-      <c r="Y249" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="250" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A250" s="3" t="s">
+      <c r="C249" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D249" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G249">
+        <v>1</v>
+      </c>
+      <c r="H249">
+        <v>1</v>
+      </c>
+      <c r="I249">
+        <v>1</v>
+      </c>
+      <c r="L249">
+        <v>1</v>
+      </c>
+      <c r="M249">
+        <v>1</v>
+      </c>
+      <c r="N249">
+        <v>1</v>
+      </c>
+      <c r="Q249">
+        <v>1</v>
+      </c>
+      <c r="R249">
+        <v>1</v>
+      </c>
+      <c r="Y249">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="250" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A250" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B250" s="3" t="s">
+      <c r="B250" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C250" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D250" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G250" s="5">
-        <v>1</v>
-      </c>
-      <c r="K250" s="5">
-        <v>1</v>
-      </c>
-      <c r="Q250" s="5">
-        <v>1</v>
-      </c>
-      <c r="R250" s="5">
-        <v>1</v>
-      </c>
-      <c r="Y250" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="251" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A251" s="3" t="s">
+      <c r="C250" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D250" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G250">
+        <v>1</v>
+      </c>
+      <c r="K250">
+        <v>1</v>
+      </c>
+      <c r="Q250">
+        <v>1</v>
+      </c>
+      <c r="R250">
+        <v>1</v>
+      </c>
+      <c r="Y250">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="251" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A251" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B251" s="3" t="s">
+      <c r="B251" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C251" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D251" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="G251" s="5">
-        <v>1</v>
-      </c>
-      <c r="I251" s="5">
-        <v>1</v>
-      </c>
-      <c r="K251" s="5">
-        <v>1</v>
-      </c>
-      <c r="N251" s="5">
-        <v>1</v>
-      </c>
-      <c r="Q251" s="5">
-        <v>1</v>
-      </c>
-      <c r="R251" s="5">
-        <v>1</v>
-      </c>
-      <c r="Y251" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="252" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A252" s="3" t="s">
+      <c r="C251" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D251" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G251">
+        <v>1</v>
+      </c>
+      <c r="I251">
+        <v>1</v>
+      </c>
+      <c r="K251">
+        <v>1</v>
+      </c>
+      <c r="N251">
+        <v>1</v>
+      </c>
+      <c r="Q251">
+        <v>1</v>
+      </c>
+      <c r="R251">
+        <v>1</v>
+      </c>
+      <c r="Y251">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="252" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A252" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B252" s="3" t="s">
+      <c r="B252" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C252" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D252" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G252" s="5">
-        <v>1</v>
-      </c>
-      <c r="H252" s="5">
-        <v>1</v>
-      </c>
-      <c r="K252" s="5">
-        <v>1</v>
-      </c>
-      <c r="M252" s="5">
-        <v>1</v>
-      </c>
-      <c r="Q252" s="5">
-        <v>1</v>
-      </c>
-      <c r="R252" s="5">
-        <v>1</v>
-      </c>
-      <c r="Y252" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="253" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A253" s="3" t="s">
+      <c r="C252" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D252" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G252">
+        <v>1</v>
+      </c>
+      <c r="H252">
+        <v>1</v>
+      </c>
+      <c r="K252">
+        <v>1</v>
+      </c>
+      <c r="M252">
+        <v>1</v>
+      </c>
+      <c r="Q252">
+        <v>1</v>
+      </c>
+      <c r="R252">
+        <v>1</v>
+      </c>
+      <c r="Y252">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="253" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A253" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B253" s="3" t="s">
+      <c r="B253" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C253" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D253" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="G253" s="5">
-        <v>1</v>
-      </c>
-      <c r="H253" s="5">
-        <v>1</v>
-      </c>
-      <c r="I253" s="5">
-        <v>1</v>
-      </c>
-      <c r="K253" s="5">
-        <v>1</v>
-      </c>
-      <c r="M253" s="5">
-        <v>1</v>
-      </c>
-      <c r="N253" s="5">
-        <v>1</v>
-      </c>
-      <c r="Q253" s="5">
-        <v>1</v>
-      </c>
-      <c r="R253" s="5">
-        <v>1</v>
-      </c>
-      <c r="Y253" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="254" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A254" s="3" t="s">
+      <c r="C253" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D253" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G253">
+        <v>1</v>
+      </c>
+      <c r="H253">
+        <v>1</v>
+      </c>
+      <c r="I253">
+        <v>1</v>
+      </c>
+      <c r="K253">
+        <v>1</v>
+      </c>
+      <c r="M253">
+        <v>1</v>
+      </c>
+      <c r="N253">
+        <v>1</v>
+      </c>
+      <c r="Q253">
+        <v>1</v>
+      </c>
+      <c r="R253">
+        <v>1</v>
+      </c>
+      <c r="Y253">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="254" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A254" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B254" s="3" t="s">
+      <c r="B254" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C254" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D254" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G254" s="5">
-        <v>1</v>
-      </c>
-      <c r="K254" s="5">
-        <v>1</v>
-      </c>
-      <c r="L254" s="5">
-        <v>1</v>
-      </c>
-      <c r="Q254" s="5">
-        <v>1</v>
-      </c>
-      <c r="R254" s="5">
-        <v>1</v>
-      </c>
-      <c r="Y254" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="255" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A255" s="3" t="s">
+      <c r="C254" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D254" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G254">
+        <v>1</v>
+      </c>
+      <c r="K254">
+        <v>1</v>
+      </c>
+      <c r="L254">
+        <v>1</v>
+      </c>
+      <c r="Q254">
+        <v>1</v>
+      </c>
+      <c r="R254">
+        <v>1</v>
+      </c>
+      <c r="Y254">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="255" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A255" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B255" s="3" t="s">
+      <c r="B255" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C255" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D255" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="G255" s="5">
-        <v>1</v>
-      </c>
-      <c r="I255" s="5">
-        <v>1</v>
-      </c>
-      <c r="K255" s="5">
-        <v>1</v>
-      </c>
-      <c r="L255" s="5">
-        <v>1</v>
-      </c>
-      <c r="N255" s="5">
-        <v>1</v>
-      </c>
-      <c r="Q255" s="5">
-        <v>1</v>
-      </c>
-      <c r="R255" s="5">
-        <v>1</v>
-      </c>
-      <c r="Y255" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="256" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A256" s="3" t="s">
+      <c r="C255" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D255" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G255">
+        <v>1</v>
+      </c>
+      <c r="I255">
+        <v>1</v>
+      </c>
+      <c r="K255">
+        <v>1</v>
+      </c>
+      <c r="L255">
+        <v>1</v>
+      </c>
+      <c r="N255">
+        <v>1</v>
+      </c>
+      <c r="Q255">
+        <v>1</v>
+      </c>
+      <c r="R255">
+        <v>1</v>
+      </c>
+      <c r="Y255">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="256" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A256" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B256" s="3" t="s">
+      <c r="B256" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C256" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D256" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G256" s="5">
-        <v>1</v>
-      </c>
-      <c r="H256" s="5">
-        <v>1</v>
-      </c>
-      <c r="K256" s="5">
-        <v>1</v>
-      </c>
-      <c r="L256" s="5">
-        <v>1</v>
-      </c>
-      <c r="M256" s="5">
-        <v>1</v>
-      </c>
-      <c r="Q256" s="5">
-        <v>1</v>
-      </c>
-      <c r="R256" s="5">
-        <v>1</v>
-      </c>
-      <c r="Y256" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="257" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A257" s="3" t="s">
+      <c r="C256" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D256" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G256">
+        <v>1</v>
+      </c>
+      <c r="H256">
+        <v>1</v>
+      </c>
+      <c r="K256">
+        <v>1</v>
+      </c>
+      <c r="L256">
+        <v>1</v>
+      </c>
+      <c r="M256">
+        <v>1</v>
+      </c>
+      <c r="Q256">
+        <v>1</v>
+      </c>
+      <c r="R256">
+        <v>1</v>
+      </c>
+      <c r="Y256">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="257" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A257" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B257" s="3" t="s">
+      <c r="B257" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C257" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D257" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="G257" s="5">
-        <v>1</v>
-      </c>
-      <c r="H257" s="5">
-        <v>1</v>
-      </c>
-      <c r="I257" s="5">
-        <v>1</v>
-      </c>
-      <c r="K257" s="5">
-        <v>1</v>
-      </c>
-      <c r="L257" s="5">
-        <v>1</v>
-      </c>
-      <c r="M257" s="5">
-        <v>1</v>
-      </c>
-      <c r="N257" s="5">
-        <v>1</v>
-      </c>
-      <c r="Q257" s="5">
-        <v>1</v>
-      </c>
-      <c r="R257" s="5">
-        <v>1</v>
-      </c>
-      <c r="Y257" s="5">
+      <c r="C257" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D257" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G257">
+        <v>1</v>
+      </c>
+      <c r="H257">
+        <v>1</v>
+      </c>
+      <c r="I257">
+        <v>1</v>
+      </c>
+      <c r="K257">
+        <v>1</v>
+      </c>
+      <c r="L257">
+        <v>1</v>
+      </c>
+      <c r="M257">
+        <v>1</v>
+      </c>
+      <c r="N257">
+        <v>1</v>
+      </c>
+      <c r="Q257">
+        <v>1</v>
+      </c>
+      <c r="R257">
+        <v>1</v>
+      </c>
+      <c r="Y257">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AB257" xr:uid="{E935C717-A0A0-4754-9512-CFF356DAFA88}"/>
+  <autoFilter ref="A1:AA257" xr:uid="{E935C717-A0A0-4754-9512-CFF356DAFA88}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Modify some control signals, fix minor errors
</commit_message>
<xml_diff>
--- a/opcode to control bits.xlsx
+++ b/opcode to control bits.xlsx
@@ -1,28 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vjrai\Documents\SC8bCPU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{452521F6-2AE8-4E72-9FB7-001723E18298}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EA8D103-272E-4016-BFFA-58C0C0F31500}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="13875" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="13875" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="v1" sheetId="1" r:id="rId1"/>
     <sheet name="v2" sheetId="2" r:id="rId2"/>
     <sheet name="v3" sheetId="3" r:id="rId3"/>
     <sheet name="v4" sheetId="4" r:id="rId4"/>
+    <sheet name="v5" sheetId="7" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'v1'!$A$1:$X$257</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'v2'!$A$1:$AA$257</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'v3'!$A$1:$AC$257</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'v4'!$A$1:$AA$257</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'v5'!$A$1:$S$1</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -45,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4270" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4797" uniqueCount="186">
   <si>
     <t>Instruction</t>
   </si>
@@ -394,6 +396,216 @@
   <si>
     <t>XORR</t>
   </si>
+  <si>
+    <t>opcode</t>
+  </si>
+  <si>
+    <t>R1/Rd/Rd1</t>
+  </si>
+  <si>
+    <t>R2/R1</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>Family</t>
+  </si>
+  <si>
+    <t>Func[8:4]/Rd2</t>
+  </si>
+  <si>
+    <t>Func[3:0]</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>CMPR</t>
+  </si>
+  <si>
+    <t>JMPR</t>
+  </si>
+  <si>
+    <t>JRALR</t>
+  </si>
+  <si>
+    <t>JPNR</t>
+  </si>
+  <si>
+    <t>JPER</t>
+  </si>
+  <si>
+    <t>JGER</t>
+  </si>
+  <si>
+    <t>JGTR</t>
+  </si>
+  <si>
+    <t>LDMU</t>
+  </si>
+  <si>
+    <t>LDW</t>
+  </si>
+  <si>
+    <t>LDH</t>
+  </si>
+  <si>
+    <t>LDB</t>
+  </si>
+  <si>
+    <t>STW</t>
+  </si>
+  <si>
+    <t>STH</t>
+  </si>
+  <si>
+    <t>STB</t>
+  </si>
+  <si>
+    <t>LDJ</t>
+  </si>
+  <si>
+    <t>Rd</t>
+  </si>
+  <si>
+    <t>ASRR</t>
+  </si>
+  <si>
+    <t>LSLR</t>
+  </si>
+  <si>
+    <t>LSRR</t>
+  </si>
+  <si>
+    <t>CSLR</t>
+  </si>
+  <si>
+    <t>CSRR</t>
+  </si>
+  <si>
+    <t>MULTD</t>
+  </si>
+  <si>
+    <t>MULTR</t>
+  </si>
+  <si>
+    <t>MULTDU</t>
+  </si>
+  <si>
+    <t>MULTRU</t>
+  </si>
+  <si>
+    <t>DIVR</t>
+  </si>
+  <si>
+    <t>DIVRU</t>
+  </si>
+  <si>
+    <t>Rd2</t>
+  </si>
+  <si>
+    <t>Rd1</t>
+  </si>
+  <si>
+    <t>JGTRU</t>
+  </si>
+  <si>
+    <t>JGERU</t>
+  </si>
+  <si>
+    <t>ADDPC</t>
+  </si>
+  <si>
+    <t>ADD_SUB</t>
+  </si>
+  <si>
+    <t>ALU_SELECT[2:0]</t>
+  </si>
+  <si>
+    <t>FLAG_WE[4:0]</t>
+  </si>
+  <si>
+    <t>REG_W_ADD_A[4:0]</t>
+  </si>
+  <si>
+    <t>REG_W_ADD_B[4:0]</t>
+  </si>
+  <si>
+    <t>REG_WE_A</t>
+  </si>
+  <si>
+    <t>REG_WE_B</t>
+  </si>
+  <si>
+    <t>REG_R_ADD_A</t>
+  </si>
+  <si>
+    <t>REG_R_ADD_B</t>
+  </si>
+  <si>
+    <t>DMEM_DLEN[1:0]</t>
+  </si>
+  <si>
+    <t>01111</t>
+  </si>
+  <si>
+    <t>Flags</t>
+  </si>
+  <si>
+    <t>10100</t>
+  </si>
+  <si>
+    <t>00100</t>
+  </si>
+  <si>
+    <t>DIVD</t>
+  </si>
+  <si>
+    <t>DIVDU</t>
+  </si>
 </sst>
 </file>
 
@@ -443,10 +655,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -22285,7 +22498,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67B22997-F6D9-4937-9D98-6675577120D6}">
   <dimension ref="A1:AA257"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="N2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -30414,4 +30627,2211 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D896E85-B550-461A-BB89-06512C5EBBCD}">
+  <dimension ref="A1:U62"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="8" ySplit="1" topLeftCell="I38" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E1" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="S62" sqref="S62"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="9.46484375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.73046875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.59765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="2.796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.9296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.19921875" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.46484375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.265625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.06640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.59765625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.9296875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.59765625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.53125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.06640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.1328125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.9296875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="6" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="U2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A3" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4" t="s">
+        <v>126</v>
+      </c>
+      <c r="P4" t="s">
+        <v>126</v>
+      </c>
+      <c r="U4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A5" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="M5" t="s">
+        <v>126</v>
+      </c>
+      <c r="P5" t="s">
+        <v>126</v>
+      </c>
+      <c r="U5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A6" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="M6" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>119</v>
+      </c>
+      <c r="U6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A7" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="L7">
+        <v>1</v>
+      </c>
+      <c r="M7" t="s">
+        <v>126</v>
+      </c>
+      <c r="N7">
+        <v>1</v>
+      </c>
+      <c r="O7" t="s">
+        <v>119</v>
+      </c>
+      <c r="P7" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>119</v>
+      </c>
+      <c r="U7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A8" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="P8" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>119</v>
+      </c>
+      <c r="U8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A9" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="J9">
+        <v>4</v>
+      </c>
+      <c r="L9">
+        <v>1</v>
+      </c>
+      <c r="M9" t="s">
+        <v>126</v>
+      </c>
+      <c r="U9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A10" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="L10">
+        <v>1</v>
+      </c>
+      <c r="M10" t="s">
+        <v>126</v>
+      </c>
+      <c r="P10" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>119</v>
+      </c>
+      <c r="U10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A11" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="L11">
+        <v>1</v>
+      </c>
+      <c r="M11" t="s">
+        <v>126</v>
+      </c>
+      <c r="P11" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>119</v>
+      </c>
+      <c r="U11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A12" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="P12" t="s">
+        <v>126</v>
+      </c>
+      <c r="T12">
+        <v>1</v>
+      </c>
+      <c r="U12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A13" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="N13">
+        <v>1</v>
+      </c>
+      <c r="O13" t="s">
+        <v>119</v>
+      </c>
+      <c r="P13" t="s">
+        <v>126</v>
+      </c>
+      <c r="T13">
+        <v>1</v>
+      </c>
+      <c r="U13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A14" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="P14" t="s">
+        <v>126</v>
+      </c>
+      <c r="T14" t="s">
+        <v>181</v>
+      </c>
+      <c r="U14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A15" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="P15" t="s">
+        <v>126</v>
+      </c>
+      <c r="T15" t="s">
+        <v>181</v>
+      </c>
+      <c r="U15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A16" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="P16" t="s">
+        <v>126</v>
+      </c>
+      <c r="T16" t="s">
+        <v>181</v>
+      </c>
+      <c r="U16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A17" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="P17" t="s">
+        <v>126</v>
+      </c>
+      <c r="T17" t="s">
+        <v>181</v>
+      </c>
+      <c r="U17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A18" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="L18">
+        <v>1</v>
+      </c>
+      <c r="M18" t="s">
+        <v>153</v>
+      </c>
+      <c r="U18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A19" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="L19">
+        <v>1</v>
+      </c>
+      <c r="M19" t="s">
+        <v>153</v>
+      </c>
+      <c r="U19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A20" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="L20">
+        <v>1</v>
+      </c>
+      <c r="M20" t="s">
+        <v>153</v>
+      </c>
+      <c r="U20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A21" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="L21">
+        <v>1</v>
+      </c>
+      <c r="M21" t="s">
+        <v>153</v>
+      </c>
+      <c r="U21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A22" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="L22">
+        <v>1</v>
+      </c>
+      <c r="M22" t="s">
+        <v>153</v>
+      </c>
+      <c r="U22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A23" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="P23" t="s">
+        <v>153</v>
+      </c>
+      <c r="U23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A24" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="P24" t="s">
+        <v>153</v>
+      </c>
+      <c r="U24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A25" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="P25" t="s">
+        <v>153</v>
+      </c>
+      <c r="U25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A26" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="J26">
+        <v>2</v>
+      </c>
+      <c r="L26">
+        <v>1</v>
+      </c>
+      <c r="M26" t="s">
+        <v>153</v>
+      </c>
+      <c r="P26" t="s">
+        <v>126</v>
+      </c>
+      <c r="U26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A27" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="T27" t="s">
+        <v>181</v>
+      </c>
+      <c r="U27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A28" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="T28" t="s">
+        <v>181</v>
+      </c>
+      <c r="U28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A29" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="T29" t="s">
+        <v>181</v>
+      </c>
+      <c r="U29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A30" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="L30">
+        <v>1</v>
+      </c>
+      <c r="M30" t="s">
+        <v>153</v>
+      </c>
+      <c r="U30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A31" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="L31">
+        <v>1</v>
+      </c>
+      <c r="M31" t="s">
+        <v>153</v>
+      </c>
+      <c r="P31" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>119</v>
+      </c>
+      <c r="S31">
+        <v>3</v>
+      </c>
+      <c r="U31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A32" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="L32">
+        <v>1</v>
+      </c>
+      <c r="M32" t="s">
+        <v>153</v>
+      </c>
+      <c r="P32" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>119</v>
+      </c>
+      <c r="U32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A33" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="I33">
+        <v>1</v>
+      </c>
+      <c r="K33" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="L33">
+        <v>1</v>
+      </c>
+      <c r="M33" t="s">
+        <v>153</v>
+      </c>
+      <c r="P33" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>119</v>
+      </c>
+      <c r="S33">
+        <v>3</v>
+      </c>
+      <c r="U33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A34" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="I34">
+        <v>1</v>
+      </c>
+      <c r="K34" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="L34">
+        <v>1</v>
+      </c>
+      <c r="M34" t="s">
+        <v>153</v>
+      </c>
+      <c r="P34" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>119</v>
+      </c>
+      <c r="U34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A35" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="J35">
+        <v>1</v>
+      </c>
+      <c r="L35">
+        <v>1</v>
+      </c>
+      <c r="M35" t="s">
+        <v>153</v>
+      </c>
+      <c r="P35" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>119</v>
+      </c>
+      <c r="S35">
+        <v>3</v>
+      </c>
+      <c r="U35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A36" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="J36">
+        <v>1</v>
+      </c>
+      <c r="L36">
+        <v>1</v>
+      </c>
+      <c r="M36" t="s">
+        <v>153</v>
+      </c>
+      <c r="P36" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>119</v>
+      </c>
+      <c r="U36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A37" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="J37">
+        <v>2</v>
+      </c>
+      <c r="L37">
+        <v>1</v>
+      </c>
+      <c r="M37" t="s">
+        <v>153</v>
+      </c>
+      <c r="P37" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>119</v>
+      </c>
+      <c r="S37">
+        <v>3</v>
+      </c>
+      <c r="U37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A38" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="J38">
+        <v>2</v>
+      </c>
+      <c r="L38">
+        <v>1</v>
+      </c>
+      <c r="M38" t="s">
+        <v>153</v>
+      </c>
+      <c r="P38" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q38" t="s">
+        <v>119</v>
+      </c>
+      <c r="U38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A39" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="J39">
+        <v>3</v>
+      </c>
+      <c r="L39">
+        <v>1</v>
+      </c>
+      <c r="M39" t="s">
+        <v>153</v>
+      </c>
+      <c r="P39" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q39" t="s">
+        <v>119</v>
+      </c>
+      <c r="S39">
+        <v>3</v>
+      </c>
+      <c r="U39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A40" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="J40">
+        <v>3</v>
+      </c>
+      <c r="L40">
+        <v>1</v>
+      </c>
+      <c r="M40" t="s">
+        <v>153</v>
+      </c>
+      <c r="P40" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q40" t="s">
+        <v>119</v>
+      </c>
+      <c r="U40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A41" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="J41">
+        <v>6</v>
+      </c>
+      <c r="L41">
+        <v>1</v>
+      </c>
+      <c r="M41" t="s">
+        <v>153</v>
+      </c>
+      <c r="P41" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q41" t="s">
+        <v>119</v>
+      </c>
+      <c r="U41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A42" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="J42">
+        <v>6</v>
+      </c>
+      <c r="L42">
+        <v>1</v>
+      </c>
+      <c r="M42" t="s">
+        <v>153</v>
+      </c>
+      <c r="P42" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q42" t="s">
+        <v>119</v>
+      </c>
+      <c r="U42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A43" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="H43" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="J43">
+        <v>5</v>
+      </c>
+      <c r="L43">
+        <v>1</v>
+      </c>
+      <c r="M43" t="s">
+        <v>153</v>
+      </c>
+      <c r="P43" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q43" t="s">
+        <v>119</v>
+      </c>
+      <c r="U43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A44" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="J44">
+        <v>5</v>
+      </c>
+      <c r="L44">
+        <v>1</v>
+      </c>
+      <c r="M44" t="s">
+        <v>153</v>
+      </c>
+      <c r="P44" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q44" t="s">
+        <v>119</v>
+      </c>
+      <c r="U44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A45" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J45">
+        <v>5</v>
+      </c>
+      <c r="L45">
+        <v>1</v>
+      </c>
+      <c r="M45" t="s">
+        <v>153</v>
+      </c>
+      <c r="P45" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q45" t="s">
+        <v>119</v>
+      </c>
+      <c r="U45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A46" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J46">
+        <v>5</v>
+      </c>
+      <c r="L46">
+        <v>1</v>
+      </c>
+      <c r="M46" t="s">
+        <v>153</v>
+      </c>
+      <c r="P46" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q46" t="s">
+        <v>119</v>
+      </c>
+      <c r="U46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A47" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="H47" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="J47">
+        <v>7</v>
+      </c>
+      <c r="L47">
+        <v>1</v>
+      </c>
+      <c r="M47" t="s">
+        <v>153</v>
+      </c>
+      <c r="P47" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q47" t="s">
+        <v>119</v>
+      </c>
+      <c r="U47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A48" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="H48" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="J48">
+        <v>7</v>
+      </c>
+      <c r="L48">
+        <v>1</v>
+      </c>
+      <c r="M48" t="s">
+        <v>153</v>
+      </c>
+      <c r="P48" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q48" t="s">
+        <v>119</v>
+      </c>
+      <c r="U48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A49" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="H49" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="J49">
+        <v>7</v>
+      </c>
+      <c r="L49">
+        <v>1</v>
+      </c>
+      <c r="M49" t="s">
+        <v>153</v>
+      </c>
+      <c r="P49" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q49" t="s">
+        <v>119</v>
+      </c>
+      <c r="U49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A50" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="H50" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="J50">
+        <v>7</v>
+      </c>
+      <c r="L50">
+        <v>1</v>
+      </c>
+      <c r="M50" t="s">
+        <v>153</v>
+      </c>
+      <c r="P50" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q50" t="s">
+        <v>119</v>
+      </c>
+      <c r="U50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A51" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="H51" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="I51">
+        <v>1</v>
+      </c>
+      <c r="K51" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="L51">
+        <v>1</v>
+      </c>
+      <c r="M51" t="s">
+        <v>166</v>
+      </c>
+      <c r="N51">
+        <v>1</v>
+      </c>
+      <c r="O51" t="s">
+        <v>165</v>
+      </c>
+      <c r="P51" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q51" t="s">
+        <v>119</v>
+      </c>
+      <c r="S51">
+        <v>3</v>
+      </c>
+      <c r="U51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A52" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="H52" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="I52">
+        <v>1</v>
+      </c>
+      <c r="K52" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="L52">
+        <v>1</v>
+      </c>
+      <c r="M52" t="s">
+        <v>166</v>
+      </c>
+      <c r="N52">
+        <v>1</v>
+      </c>
+      <c r="O52" t="s">
+        <v>165</v>
+      </c>
+      <c r="P52" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q52" t="s">
+        <v>119</v>
+      </c>
+      <c r="U52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A53" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="H53" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="K53" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="L53">
+        <v>1</v>
+      </c>
+      <c r="M53" t="s">
+        <v>166</v>
+      </c>
+      <c r="N53">
+        <v>1</v>
+      </c>
+      <c r="O53" t="s">
+        <v>165</v>
+      </c>
+      <c r="P53" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q53" t="s">
+        <v>119</v>
+      </c>
+      <c r="S53">
+        <v>3</v>
+      </c>
+      <c r="U53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A54" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="H54" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="K54" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="L54">
+        <v>1</v>
+      </c>
+      <c r="M54" t="s">
+        <v>166</v>
+      </c>
+      <c r="N54">
+        <v>1</v>
+      </c>
+      <c r="O54" t="s">
+        <v>165</v>
+      </c>
+      <c r="P54" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q54" t="s">
+        <v>119</v>
+      </c>
+      <c r="U54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A55" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="H55" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="I55">
+        <v>1</v>
+      </c>
+      <c r="K55" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="L55">
+        <v>1</v>
+      </c>
+      <c r="M55" t="s">
+        <v>166</v>
+      </c>
+      <c r="N55">
+        <v>1</v>
+      </c>
+      <c r="O55" t="s">
+        <v>165</v>
+      </c>
+      <c r="P55" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q55" t="s">
+        <v>119</v>
+      </c>
+      <c r="S55">
+        <v>3</v>
+      </c>
+      <c r="U55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A56" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="H56" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="I56">
+        <v>1</v>
+      </c>
+      <c r="K56" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="L56">
+        <v>1</v>
+      </c>
+      <c r="M56" t="s">
+        <v>166</v>
+      </c>
+      <c r="N56">
+        <v>1</v>
+      </c>
+      <c r="O56" t="s">
+        <v>165</v>
+      </c>
+      <c r="P56" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q56" t="s">
+        <v>119</v>
+      </c>
+      <c r="U56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A57" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="H57" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="K57" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="L57">
+        <v>1</v>
+      </c>
+      <c r="M57" t="s">
+        <v>166</v>
+      </c>
+      <c r="N57">
+        <v>1</v>
+      </c>
+      <c r="O57" t="s">
+        <v>165</v>
+      </c>
+      <c r="P57" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q57" t="s">
+        <v>119</v>
+      </c>
+      <c r="S57">
+        <v>3</v>
+      </c>
+      <c r="U57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A58" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="H58" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="K58" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="L58">
+        <v>1</v>
+      </c>
+      <c r="M58" t="s">
+        <v>166</v>
+      </c>
+      <c r="N58">
+        <v>1</v>
+      </c>
+      <c r="O58" t="s">
+        <v>165</v>
+      </c>
+      <c r="P58" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q58" t="s">
+        <v>119</v>
+      </c>
+      <c r="U58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A59" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="H59" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="P59" t="s">
+        <v>126</v>
+      </c>
+      <c r="T59" t="s">
+        <v>181</v>
+      </c>
+      <c r="U59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A60" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="H60" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="P60" t="s">
+        <v>126</v>
+      </c>
+      <c r="T60" t="s">
+        <v>181</v>
+      </c>
+      <c r="U60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A61" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="H61" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="I61">
+        <v>1</v>
+      </c>
+      <c r="K61" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="P61" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q61" t="s">
+        <v>119</v>
+      </c>
+      <c r="S61">
+        <v>3</v>
+      </c>
+      <c r="U61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A62" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="H62" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="L62">
+        <v>1</v>
+      </c>
+      <c r="M62" t="s">
+        <v>153</v>
+      </c>
+      <c r="P62" t="s">
+        <v>126</v>
+      </c>
+      <c r="U62">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>